<commit_message>
changed URL parameter name;added fvp description
</commit_message>
<xml_diff>
--- a/ToTaL Test Cases.xlsx
+++ b/ToTaL Test Cases.xlsx
@@ -603,15 +603,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -628,6 +619,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -933,8 +933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15:C16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -960,10 +960,10 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="5" t="s">
         <v>112</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -980,10 +980,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -991,8 +991,8 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="10"/>
-      <c r="B3" s="6" t="s">
+      <c r="A3" s="7"/>
+      <c r="B3" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -1000,8 +1000,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="10"/>
-      <c r="B4" s="6" t="s">
+      <c r="A4" s="7"/>
+      <c r="B4" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -1009,8 +1009,8 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="10"/>
-      <c r="B5" s="6" t="s">
+      <c r="A5" s="7"/>
+      <c r="B5" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -1018,8 +1018,8 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="10"/>
-      <c r="B6" s="6" t="s">
+      <c r="A6" s="7"/>
+      <c r="B6" s="3" t="s">
         <v>29</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -1027,8 +1027,8 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="10"/>
-      <c r="B7" s="6" t="s">
+      <c r="A7" s="7"/>
+      <c r="B7" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -1036,8 +1036,8 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="10"/>
-      <c r="B8" s="6" t="s">
+      <c r="A8" s="7"/>
+      <c r="B8" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -1045,8 +1045,8 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="10"/>
-      <c r="B9" s="6" t="s">
+      <c r="A9" s="7"/>
+      <c r="B9" s="3" t="s">
         <v>32</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -1054,8 +1054,8 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="10"/>
-      <c r="B10" s="6" t="s">
+      <c r="A10" s="7"/>
+      <c r="B10" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -1063,8 +1063,8 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="10"/>
-      <c r="B11" s="6" t="s">
+      <c r="A11" s="7"/>
+      <c r="B11" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -1072,8 +1072,8 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="10"/>
-      <c r="B12" s="6" t="s">
+      <c r="A12" s="7"/>
+      <c r="B12" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -1081,8 +1081,8 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="10"/>
-      <c r="B13" s="6" t="s">
+      <c r="A13" s="7"/>
+      <c r="B13" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -1090,8 +1090,8 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="11"/>
-      <c r="B14" s="6" t="s">
+      <c r="A14" s="8"/>
+      <c r="B14" s="3" t="s">
         <v>37</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -1099,10 +1099,10 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="3" t="s">
         <v>38</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -1110,8 +1110,8 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="4"/>
-      <c r="B16" s="6" t="s">
+      <c r="A16" s="10"/>
+      <c r="B16" s="3" t="s">
         <v>39</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -1119,8 +1119,8 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A17" s="4"/>
-      <c r="B17" s="6" t="s">
+      <c r="A17" s="10"/>
+      <c r="B17" s="3" t="s">
         <v>40</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -1128,8 +1128,8 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="5"/>
-      <c r="B18" s="6" t="s">
+      <c r="A18" s="11"/>
+      <c r="B18" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C18" s="2" t="s">
@@ -1137,10 +1137,10 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="3" t="s">
         <v>46</v>
       </c>
       <c r="C19" s="2" t="s">
@@ -1148,8 +1148,8 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="4"/>
-      <c r="B20" s="6" t="s">
+      <c r="A20" s="10"/>
+      <c r="B20" s="3" t="s">
         <v>47</v>
       </c>
       <c r="C20" s="2" t="s">
@@ -1157,8 +1157,8 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="5"/>
-      <c r="B21" s="6" t="s">
+      <c r="A21" s="11"/>
+      <c r="B21" s="3" t="s">
         <v>48</v>
       </c>
       <c r="C21" s="2" t="s">
@@ -1166,10 +1166,10 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C22" s="2" t="s">
@@ -1177,8 +1177,8 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A23" s="4"/>
-      <c r="B23" s="6" t="s">
+      <c r="A23" s="10"/>
+      <c r="B23" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C23" s="2" t="s">
@@ -1186,8 +1186,8 @@
       </c>
     </row>
     <row r="24" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24" s="4"/>
-      <c r="B24" s="6" t="s">
+      <c r="A24" s="10"/>
+      <c r="B24" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C24" s="2" t="s">
@@ -1195,8 +1195,8 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A25" s="5"/>
-      <c r="B25" s="6" t="s">
+      <c r="A25" s="11"/>
+      <c r="B25" s="3" t="s">
         <v>57</v>
       </c>
       <c r="C25" s="2" t="s">
@@ -1204,10 +1204,10 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="3" t="s">
         <v>66</v>
       </c>
       <c r="C26" s="2" t="s">
@@ -1215,8 +1215,8 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="5"/>
-      <c r="B27" s="6" t="s">
+      <c r="A27" s="11"/>
+      <c r="B27" s="3" t="s">
         <v>67</v>
       </c>
       <c r="C27" s="2" t="s">
@@ -1224,10 +1224,10 @@
       </c>
     </row>
     <row r="28" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="3" t="s">
         <v>68</v>
       </c>
       <c r="C28" s="2" t="s">
@@ -1235,8 +1235,8 @@
       </c>
     </row>
     <row r="29" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A29" s="4"/>
-      <c r="B29" s="6" t="s">
+      <c r="A29" s="10"/>
+      <c r="B29" s="3" t="s">
         <v>69</v>
       </c>
       <c r="C29" s="2" t="s">
@@ -1244,8 +1244,8 @@
       </c>
     </row>
     <row r="30" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A30" s="4"/>
-      <c r="B30" s="6" t="s">
+      <c r="A30" s="10"/>
+      <c r="B30" s="3" t="s">
         <v>70</v>
       </c>
       <c r="C30" s="2" t="s">
@@ -1253,8 +1253,8 @@
       </c>
     </row>
     <row r="31" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A31" s="5"/>
-      <c r="B31" s="6" t="s">
+      <c r="A31" s="11"/>
+      <c r="B31" s="3" t="s">
         <v>71</v>
       </c>
       <c r="C31" s="2" t="s">
@@ -1262,10 +1262,10 @@
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="3" t="s">
         <v>80</v>
       </c>
       <c r="C32" s="2" t="s">
@@ -1273,8 +1273,8 @@
       </c>
     </row>
     <row r="33" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="5"/>
-      <c r="B33" s="6" t="s">
+      <c r="A33" s="11"/>
+      <c r="B33" s="3" t="s">
         <v>81</v>
       </c>
       <c r="C33" s="2" t="s">
@@ -1282,10 +1282,10 @@
       </c>
     </row>
     <row r="34" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="3" t="s">
         <v>82</v>
       </c>
       <c r="C34" s="2" t="s">
@@ -1293,8 +1293,8 @@
       </c>
     </row>
     <row r="35" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A35" s="4"/>
-      <c r="B35" s="6" t="s">
+      <c r="A35" s="10"/>
+      <c r="B35" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C35" s="2" t="s">
@@ -1302,8 +1302,8 @@
       </c>
     </row>
     <row r="36" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A36" s="4"/>
-      <c r="B36" s="6" t="s">
+      <c r="A36" s="10"/>
+      <c r="B36" s="3" t="s">
         <v>84</v>
       </c>
       <c r="C36" s="2" t="s">
@@ -1311,8 +1311,8 @@
       </c>
     </row>
     <row r="37" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A37" s="5"/>
-      <c r="B37" s="6" t="s">
+      <c r="A37" s="11"/>
+      <c r="B37" s="3" t="s">
         <v>85</v>
       </c>
       <c r="C37" s="2" t="s">
@@ -1320,10 +1320,10 @@
       </c>
     </row>
     <row r="38" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="3" t="s">
         <v>99</v>
       </c>
       <c r="C38" s="2" t="s">
@@ -1331,8 +1331,8 @@
       </c>
     </row>
     <row r="39" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A39" s="4"/>
-      <c r="B39" s="6" t="s">
+      <c r="A39" s="10"/>
+      <c r="B39" s="3" t="s">
         <v>100</v>
       </c>
       <c r="C39" s="2" t="s">
@@ -1340,8 +1340,8 @@
       </c>
     </row>
     <row r="40" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="4"/>
-      <c r="B40" s="6" t="s">
+      <c r="A40" s="10"/>
+      <c r="B40" s="3" t="s">
         <v>101</v>
       </c>
       <c r="C40" s="2" t="s">
@@ -1349,8 +1349,8 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A41" s="4"/>
-      <c r="B41" s="6" t="s">
+      <c r="A41" s="10"/>
+      <c r="B41" s="3" t="s">
         <v>102</v>
       </c>
       <c r="C41" s="2" t="s">
@@ -1358,8 +1358,8 @@
       </c>
     </row>
     <row r="42" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A42" s="4"/>
-      <c r="B42" s="6" t="s">
+      <c r="A42" s="10"/>
+      <c r="B42" s="3" t="s">
         <v>103</v>
       </c>
       <c r="C42" s="2" t="s">
@@ -1367,8 +1367,8 @@
       </c>
     </row>
     <row r="43" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A43" s="4"/>
-      <c r="B43" s="6" t="s">
+      <c r="A43" s="10"/>
+      <c r="B43" s="3" t="s">
         <v>104</v>
       </c>
       <c r="C43" s="2" t="s">
@@ -1376,8 +1376,8 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A44" s="5"/>
-      <c r="B44" s="6" t="s">
+      <c r="A44" s="11"/>
+      <c r="B44" s="3" t="s">
         <v>105</v>
       </c>
       <c r="C44" s="2" t="s">
@@ -1385,10 +1385,10 @@
       </c>
     </row>
     <row r="45" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A45" s="3" t="s">
+      <c r="A45" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="B45" s="3" t="s">
         <v>106</v>
       </c>
       <c r="C45" s="2" t="s">
@@ -1396,8 +1396,8 @@
       </c>
     </row>
     <row r="46" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A46" s="4"/>
-      <c r="B46" s="6" t="s">
+      <c r="A46" s="10"/>
+      <c r="B46" s="3" t="s">
         <v>107</v>
       </c>
       <c r="C46" s="2" t="s">
@@ -1405,8 +1405,8 @@
       </c>
     </row>
     <row r="47" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A47" s="4"/>
-      <c r="B47" s="6" t="s">
+      <c r="A47" s="10"/>
+      <c r="B47" s="3" t="s">
         <v>108</v>
       </c>
       <c r="C47" s="2" t="s">
@@ -1414,8 +1414,8 @@
       </c>
     </row>
     <row r="48" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A48" s="5"/>
-      <c r="B48" s="6" t="s">
+      <c r="A48" s="11"/>
+      <c r="B48" s="3" t="s">
         <v>109</v>
       </c>
       <c r="C48" s="2" t="s">
@@ -1423,199 +1423,199 @@
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B49" s="6"/>
+      <c r="B49" s="3"/>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B50" s="6"/>
+      <c r="B50" s="3"/>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B51" s="6"/>
+      <c r="B51" s="3"/>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B52" s="6"/>
+      <c r="B52" s="3"/>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B53" s="6"/>
+      <c r="B53" s="3"/>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B54" s="6"/>
+      <c r="B54" s="3"/>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B55" s="6"/>
+      <c r="B55" s="3"/>
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B56" s="6"/>
+      <c r="B56" s="3"/>
     </row>
     <row r="57" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B57" s="6"/>
+      <c r="B57" s="3"/>
     </row>
     <row r="58" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B58" s="6"/>
+      <c r="B58" s="3"/>
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B59" s="6"/>
+      <c r="B59" s="3"/>
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B60" s="6"/>
+      <c r="B60" s="3"/>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B61" s="6"/>
+      <c r="B61" s="3"/>
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B62" s="6"/>
+      <c r="B62" s="3"/>
     </row>
     <row r="63" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B63" s="6"/>
+      <c r="B63" s="3"/>
     </row>
     <row r="64" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B64" s="6"/>
+      <c r="B64" s="3"/>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B65" s="6"/>
+      <c r="B65" s="3"/>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B66" s="6"/>
+      <c r="B66" s="3"/>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B67" s="6"/>
+      <c r="B67" s="3"/>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B68" s="6"/>
+      <c r="B68" s="3"/>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B69" s="6"/>
+      <c r="B69" s="3"/>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B70" s="6"/>
+      <c r="B70" s="3"/>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B71" s="6"/>
+      <c r="B71" s="3"/>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B72" s="6"/>
+      <c r="B72" s="3"/>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B73" s="6"/>
+      <c r="B73" s="3"/>
     </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B74" s="6"/>
+      <c r="B74" s="3"/>
     </row>
     <row r="75" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B75" s="6"/>
+      <c r="B75" s="3"/>
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B76" s="6"/>
+      <c r="B76" s="3"/>
     </row>
     <row r="77" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B77" s="6"/>
+      <c r="B77" s="3"/>
     </row>
     <row r="78" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B78" s="6"/>
+      <c r="B78" s="3"/>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B79" s="6"/>
+      <c r="B79" s="3"/>
     </row>
     <row r="80" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B80" s="6"/>
+      <c r="B80" s="3"/>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B81" s="6"/>
+      <c r="B81" s="3"/>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B82" s="6"/>
+      <c r="B82" s="3"/>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B83" s="6"/>
+      <c r="B83" s="3"/>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B84" s="6"/>
+      <c r="B84" s="3"/>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B85" s="6"/>
+      <c r="B85" s="3"/>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B86" s="6"/>
+      <c r="B86" s="3"/>
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B87" s="6"/>
+      <c r="B87" s="3"/>
     </row>
     <row r="88" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B88" s="6"/>
+      <c r="B88" s="3"/>
     </row>
     <row r="89" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B89" s="6"/>
+      <c r="B89" s="3"/>
     </row>
     <row r="90" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B90" s="6"/>
+      <c r="B90" s="3"/>
     </row>
     <row r="91" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B91" s="6"/>
+      <c r="B91" s="3"/>
     </row>
     <row r="92" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B92" s="6"/>
+      <c r="B92" s="3"/>
     </row>
     <row r="93" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B93" s="6"/>
+      <c r="B93" s="3"/>
     </row>
     <row r="94" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B94" s="6"/>
+      <c r="B94" s="3"/>
     </row>
     <row r="95" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B95" s="6"/>
+      <c r="B95" s="3"/>
     </row>
     <row r="96" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B96" s="6"/>
+      <c r="B96" s="3"/>
     </row>
     <row r="97" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B97" s="6"/>
+      <c r="B97" s="3"/>
     </row>
     <row r="98" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B98" s="6"/>
+      <c r="B98" s="3"/>
     </row>
     <row r="99" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B99" s="6"/>
+      <c r="B99" s="3"/>
     </row>
     <row r="100" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B100" s="6"/>
+      <c r="B100" s="3"/>
     </row>
     <row r="101" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B101" s="6"/>
+      <c r="B101" s="3"/>
     </row>
     <row r="102" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B102" s="6"/>
+      <c r="B102" s="3"/>
     </row>
     <row r="103" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B103" s="6"/>
+      <c r="B103" s="3"/>
     </row>
     <row r="104" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B104" s="6"/>
+      <c r="B104" s="3"/>
     </row>
     <row r="105" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B105" s="6"/>
+      <c r="B105" s="3"/>
     </row>
     <row r="106" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B106" s="6"/>
+      <c r="B106" s="3"/>
     </row>
     <row r="107" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B107" s="6"/>
+      <c r="B107" s="3"/>
     </row>
     <row r="108" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B108" s="6"/>
+      <c r="B108" s="3"/>
     </row>
     <row r="109" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B109" s="6"/>
+      <c r="B109" s="3"/>
     </row>
     <row r="110" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B110" s="6"/>
+      <c r="B110" s="3"/>
     </row>
     <row r="111" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B111" s="6"/>
+      <c r="B111" s="3"/>
     </row>
     <row r="112" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B112" s="6"/>
+      <c r="B112" s="3"/>
     </row>
     <row r="113" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B113" s="6"/>
+      <c r="B113" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>

<commit_message>
added verifying URL function
</commit_message>
<xml_diff>
--- a/ToTaL Test Cases.xlsx
+++ b/ToTaL Test Cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="162">
   <si>
     <t>Test Cases</t>
   </si>
@@ -36,113 +36,9 @@
     <t xml:space="preserve">Automation Execution </t>
   </si>
   <si>
-    <t>Verify if groupBy parameter is set to FAC,
-area parameter is set to ASSY,
-perspective parameter is set to FAB,
-time parameter is set to 0,
-tranDate parameter is set to startDate-endDate
-then API will return a tabular data based on the filter values applied.</t>
-  </si>
-  <si>
     <t>groupBy (positive)</t>
   </si>
   <si>
-    <t>Verify if groupBy parameter is set to LOC,
-area parameter is set to ASSY,
-perspective parameter is set to FAB,
-time parameter is set to 0,
-tranDate parameter is set to startDate-endDate
-then API will return a tabular data based on the filter values applied.</t>
-  </si>
-  <si>
-    <t>Verify if groupBy parameter is set to PRTECH,
-area parameter is set to ASSY,
-perspective parameter is set to FAB,
-time parameter is set to 0,
-tranDate parameter is set to startDate-endDate
-then API will return a tabular data based on the filter values applied.</t>
-  </si>
-  <si>
-    <t>Verify if groupBy parameter is set to TECH,
-area parameter is set to ASSY,
-perspective parameter is set to FAB,
-time parameter is set to 0,
-tranDate parameter is set to startDate-endDate
-then API will return a tabular data based on the filter values applied.</t>
-  </si>
-  <si>
-    <t>Verify if groupBy parameter is set to CTECH,
-area parameter is set to ASSY,
-perspective parameter is set to FAB,
-time parameter is set to 0,
-tranDate parameter is set to startDate-endDate
-then API will return a tabular data based on the filter values applied.</t>
-  </si>
-  <si>
-    <t>Verify if groupBy parameter is set to SBE,
-area parameter is set to ASSY,
-perspective parameter is set to FAB,
-time parameter is set to 0,
-tranDate parameter is set to startDate-endDate
-then API will return a tabular data based on the filter values applied.</t>
-  </si>
-  <si>
-    <t>Verify if groupBy parameter is set to SBE_1,
-area parameter is set to ASSY,
-perspective parameter is set to FAB,
-time parameter is set to 0,
-tranDate parameter is set to startDate-endDate
-then API will return a tabular data based on the filter values applied.</t>
-  </si>
-  <si>
-    <t>Verify if groupBy parameter is set to SBE_2,
-area parameter is set to ASSY,
-perspective parameter is set to FAB,
-time parameter is set to 0,
-tranDate parameter is set to startDate-endDate
-then API will return a tabular data based on the filter values applied.</t>
-  </si>
-  <si>
-    <t>Verify if groupBy parameter is set to MATERIAL,
-area parameter is set to ASSY,
-perspective parameter is set to FAB,
-time parameter is set to 0,
-tranDate parameter is set to startDate-endDate
-then API will return a tabular data based on the filter values applied.</t>
-  </si>
-  <si>
-    <t>Verify if groupBy parameter is set to DEVICE,
-area parameter is set to ASSY,
-perspective parameter is set to FAB,
-time parameter is set to 0,
-tranDate parameter is set to startDate-endDate
-then API will return a tabular data based on the filter values applied.</t>
-  </si>
-  <si>
-    <t>Verify if groupBy parameter is set to CHIP,
-area parameter is set to ASSY,
-perspective parameter is set to FAB,
-time parameter is set to 0,
-tranDate parameter is set to startDate-endDate
-then API will return a tabular data based on the filter values applied.</t>
-  </si>
-  <si>
-    <t>Verify if groupBy parameter is set to FABLOT,
-area parameter is set to ASSY,
-perspective parameter is set to FAB,
-time parameter is set to 0,
-tranDate parameter is set to startDate-endDate
-then API will return a tabular data based on the filter values applied.</t>
-  </si>
-  <si>
-    <t>Verify if groupBy parameter is set to LOT,
-area parameter is set to ASSY,
-perspective parameter is set to FAB,
-time parameter is set to 0,
-tranDate parameter is set to startDate-endDate
-then API will return a tabular data based on the filter values applied.</t>
-  </si>
-  <si>
     <t>groupBy (negative)</t>
   </si>
   <si>
@@ -212,30 +108,6 @@
     <t>area (positive)</t>
   </si>
   <si>
-    <t>Verify if area parameter is set to TEST,
-groupBy parameter is set to FAC,
-perspective parameter is set to FAB,
-time parameter is set to 0,
-tranDate parameter is set to startDate-endDate
-then API will return a tabular data based on the filter values applied.</t>
-  </si>
-  <si>
-    <t>Verify if area parameter is set to SORT,
-groupBy parameter is set to FAC,
-perspective parameter is set to FAB,
-time parameter is set to 0,
-tranDate parameter is set to startDate-endDate
-then API will return a tabular data based on the filter values applied.</t>
-  </si>
-  <si>
-    <t>Verify if area parameter is set to FAB,
-groupBy parameter is set to FAC,
-perspective parameter is set to FAB,
-time parameter is set to 0,
-tranDate parameter is set to startDate-endDate
-then API will return a tabular data based on the filter values applied.</t>
-  </si>
-  <si>
     <t>areaPos_tc_001</t>
   </si>
   <si>
@@ -275,17 +147,6 @@
     <t>persepctive (positive)</t>
   </si>
   <si>
-    <t>Verify if Fab is the default value of perspective parameter.</t>
-  </si>
-  <si>
-    <t>Verify if perspective parameter is set to AT,
-area parameter is set to FAB,
-groupBy parameter is set to FAC,
-time parameter is set to 0,
-tranDate parameter is set to startDate-endDate
-then API will return a tabular data based on the filter values applied.</t>
-  </si>
-  <si>
     <t>Verify if perspective parameter is set to null then API will return an error message.</t>
   </si>
   <si>
@@ -319,20 +180,6 @@
     <t>persNeg_tc_004</t>
   </si>
   <si>
-    <t>Verify if dallas is the  default value of time parameter.</t>
-  </si>
-  <si>
-    <t>Verify if time parameter is set to 1,
-perspective parameter is set to AT,
-area parameter is set to FAB,
-groupBy parameter is set to FAC,
-tranDate parameter is set to startDate-endDate
-then API will return a tabular data based on the filter values applied.</t>
-  </si>
-  <si>
-    <t>time (positive)</t>
-  </si>
-  <si>
     <t>Verify if time parameter is set to null then API will return an error message.</t>
   </si>
   <si>
@@ -369,62 +216,6 @@
     <t>tranDate (positive)</t>
   </si>
   <si>
-    <t>Verify if tranDate parameter is set to LM,
-time parameter is set to 0,
-perspective parameter is set to AT,
-area parameter is set to FAB,
-groupBy parameter is set to FAC,
-then API will return a tabular data based on the filter values applied.</t>
-  </si>
-  <si>
-    <t>Verify if tranDate parameter is set to L30D,
-time parameter is set to 0,
-perspective parameter is set to AT,
-area parameter is set to FAB,
-groupBy parameter is set to FAC,
-then API will return a tabular data based on the filter values applied.</t>
-  </si>
-  <si>
-    <t>Verify if tranDate parameter is set to L90D,
-time parameter is set to 0,
-perspective parameter is set to AT,
-area parameter is set to FAB,
-groupBy parameter is set to FAC,
-then API will return a tabular data based on the filter values applied.</t>
-  </si>
-  <si>
-    <t>Verify if tranDate parameter is set to LQ,
-time parameter is set to 0,
-perspective parameter is set to AT,
-area parameter is set to FAB,
-groupBy parameter is set to FAC,
-then API will return a tabular data based on the filter values applied.</t>
-  </si>
-  <si>
-    <t>Verify if tranDate parameter is set to MTD,
-time parameter is set to 0,
-perspective parameter is set to AT,
-area parameter is set to FAB,
-groupBy parameter is set to FAC,
-then API will return a tabular data based on the filter values applied.</t>
-  </si>
-  <si>
-    <t>Verify if tranDate parameter is set to QTD,
-time parameter is set to 0,
-perspective parameter is set to AT,
-area parameter is set to FAB,
-groupBy parameter is set to FAC,
-then API will return a tabular data based on the filter values applied.</t>
-  </si>
-  <si>
-    <t>Verify if tranDate parameter is set to YTD,
-time parameter is set to 0,
-perspective parameter is set to AT,
-area parameter is set to FAB,
-groupBy parameter is set to FAC,
-then API will return a tabular data based on the filter values applied.</t>
-  </si>
-  <si>
     <t>Verify if tranDate parameter is set to null then API will return an error message.</t>
   </si>
   <si>
@@ -480,6 +271,237 @@
   </si>
   <si>
     <t xml:space="preserve">Date of script automation </t>
+  </si>
+  <si>
+    <t>Verify if groupBy parameter is set to FAC then API will return a tabular data based on the filter values applied.</t>
+  </si>
+  <si>
+    <t>Verify if groupBy parameter is set to LOC, then API will return a tabular data based on the filter values applied.</t>
+  </si>
+  <si>
+    <t>Verify if groupBy parameter is set to PRTECH, then API will return a tabular data based on the filter values applied.</t>
+  </si>
+  <si>
+    <t>Verify if groupBy parameter is set to TECH, then API will return a tabular data based on the filter values applied.</t>
+  </si>
+  <si>
+    <t>Verify if groupBy parameter is set to CTECH, then API will return a tabular data based on the filter values applied.</t>
+  </si>
+  <si>
+    <t>Verify if groupBy parameter is set to SBE, then API will return a tabular data based on the filter values applied.</t>
+  </si>
+  <si>
+    <t>Verify if groupBy parameter is set to SBE_1, then API will return a tabular data based on the filter values applied.</t>
+  </si>
+  <si>
+    <t>Verify if groupBy parameter is set to SBE_2, then API will return a tabular data based on the filter values applied.</t>
+  </si>
+  <si>
+    <t>Verify if groupBy parameter is set to MATERIAL, then API will return a tabular data based on the filter values applied.</t>
+  </si>
+  <si>
+    <t>Verify if groupBy parameter is set to DEVICE, then API will return a tabular data based on the filter values applied.</t>
+  </si>
+  <si>
+    <t>Verify if groupBy parameter is set to CHIP, then API will return a tabular data based on the filter values applied.</t>
+  </si>
+  <si>
+    <t>Verify if groupBy parameter is set to FABLOT, then API will return a tabular data based on the filter values applied.</t>
+  </si>
+  <si>
+    <t>Verify if area parameter is set to TEST, then API will return a tabular data based on the filter values applied.</t>
+  </si>
+  <si>
+    <t>Verify if area parameter is set to SORT, then API will return a tabular data based on the filter values applied.</t>
+  </si>
+  <si>
+    <t>Verify if area parameter is set to FAB, then API will return a tabular data based on the filter values applied.</t>
+  </si>
+  <si>
+    <t>Verify if groupBy parameter is set to LOT, then API will return a tabular data based on the filter values applied.</t>
+  </si>
+  <si>
+    <t>Verify if time parameter is set to 1, then API will return a tabular data based on the filter values applied.</t>
+  </si>
+  <si>
+    <t>local (positive)</t>
+  </si>
+  <si>
+    <t>Verify if local is set to dallas, then API will return a tabular data based on the filter values applied.</t>
+  </si>
+  <si>
+    <t>Verify if tranDate parameter is set to L30D, then API will return a tabular data based on the filter values applied.</t>
+  </si>
+  <si>
+    <t>Verify if tranDate parameter is set to LM, then API will return a tabular data based on the filter values applied.</t>
+  </si>
+  <si>
+    <t>Verify if tranDate parameter is set to LQ, then API will return a tabular data based on the filter values applied.</t>
+  </si>
+  <si>
+    <t>Verify if tranDate parameter is set to MTD,then API will return a tabular data based on the filter values applied.</t>
+  </si>
+  <si>
+    <t>Verify if tranDate parameter is set to QTD, then API will return a tabular data based on the filter values applied.</t>
+  </si>
+  <si>
+    <t>Verify if tranDate parameter is set to YTD, then API will return a tabular data based on the filter values applied.</t>
+  </si>
+  <si>
+    <t>Verify if tranDate parameter is set to 20200318-20200523, then API will return a tabular data based on the filter values applied.</t>
+  </si>
+  <si>
+    <t>prtech (positive)</t>
+  </si>
+  <si>
+    <t>prtechPos_tc_001</t>
+  </si>
+  <si>
+    <t>tech (positive)</t>
+  </si>
+  <si>
+    <t>techPos_tc_001</t>
+  </si>
+  <si>
+    <t>ctech (positive)</t>
+  </si>
+  <si>
+    <t>ctechPos_tc_001</t>
+  </si>
+  <si>
+    <t>sbe (positive)</t>
+  </si>
+  <si>
+    <t>sbePos_tc_001</t>
+  </si>
+  <si>
+    <t>sbe1 (positive)</t>
+  </si>
+  <si>
+    <t>sbe2 (positive)</t>
+  </si>
+  <si>
+    <t>sbe1Pos_tc_001</t>
+  </si>
+  <si>
+    <t>sbe2Pos_tc_001</t>
+  </si>
+  <si>
+    <t>device (positive)</t>
+  </si>
+  <si>
+    <t>devicePos_tc_001</t>
+  </si>
+  <si>
+    <t>material (positive)</t>
+  </si>
+  <si>
+    <t>materialPos_tc_001</t>
+  </si>
+  <si>
+    <t>chipname (positive)</t>
+  </si>
+  <si>
+    <t>chipnamePos_tc_001</t>
+  </si>
+  <si>
+    <t>fablot (positive)</t>
+  </si>
+  <si>
+    <t>fablotPos_tc_001</t>
+  </si>
+  <si>
+    <t>lot (positive)</t>
+  </si>
+  <si>
+    <t>lotPos_tc_001</t>
+  </si>
+  <si>
+    <t>columns (positive)</t>
+  </si>
+  <si>
+    <t>columnsPos_tc_001</t>
+  </si>
+  <si>
+    <t>fabLocation (positive)</t>
+  </si>
+  <si>
+    <t>fabLocationPos_tc_001</t>
+  </si>
+  <si>
+    <t>fabFacility (positive)</t>
+  </si>
+  <si>
+    <t>fabFacilityPos_tc_001</t>
+  </si>
+  <si>
+    <t>probeLocation (positive)</t>
+  </si>
+  <si>
+    <t>probeLocationPos_tc_001</t>
+  </si>
+  <si>
+    <t>probeFacility (positive)</t>
+  </si>
+  <si>
+    <t>probeFacilityPos_tc_001</t>
+  </si>
+  <si>
+    <t>Verify if device parameter is set, then API will return a tabular data based on the filter values applied.</t>
+  </si>
+  <si>
+    <t>Verify if material parameter is set, then API will return a tabular data based on the filter values applied.</t>
+  </si>
+  <si>
+    <t>Verify if chipname parameter is set, then API will return a tabular data based on the filter values applied.</t>
+  </si>
+  <si>
+    <t>Verify if fablot parameter is set, then API will return a tabular data based on the filter values applied.</t>
+  </si>
+  <si>
+    <t>Verify if lot parameter is set, then API will return a tabular data based on the filter values applied.</t>
+  </si>
+  <si>
+    <t>Verify if columns parameter is set, then API will return a tabular data based on the filter values applied.</t>
+  </si>
+  <si>
+    <t>Verify if sbe1 parameter is set, then API will return a tabular data based on the filter values applied.</t>
+  </si>
+  <si>
+    <t>Verify if sbe2 parameter is set, then API will return a tabular data based on the filter values applied.</t>
+  </si>
+  <si>
+    <t>Verify if sbe parameter is set, then API will return a tabular data based on the filter values applied.</t>
+  </si>
+  <si>
+    <t>Verify if ctech parameter is set, then API will return a tabular data based on the filter values applied.</t>
+  </si>
+  <si>
+    <t>Verify if tech parameter is set, then API will return a tabular data based on the filter values applied.</t>
+  </si>
+  <si>
+    <t>Verify if prtech parameter is set, then API will return a tabular data based on the filter values applied.</t>
+  </si>
+  <si>
+    <t>Verify if probeLocation parameter is set, then API will return a tabular data based on the filter values applied.</t>
+  </si>
+  <si>
+    <t>Verify if probeFacility parameter is set, then API will return a tabular data based on the filter values applied.</t>
+  </si>
+  <si>
+    <t>Verify if fabLocation parameter is set, then API will return a tabular data based on the filter values applied.</t>
+  </si>
+  <si>
+    <t>Verify if perspective parameter is set to AT,then API will return a tabular data based on the filter values applied.</t>
+  </si>
+  <si>
+    <t>Verify if perspective parameter is set to FAB,then API will return a tabular data based on the filter values applied.</t>
+  </si>
+  <si>
+    <t>Verify if area parameter is set to ASSY, then API will return a tabular data based on the filter values applied.</t>
+  </si>
+  <si>
+    <t>areaPos_tc_004</t>
   </si>
 </sst>
 </file>
@@ -595,7 +617,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -629,6 +651,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -931,17 +956,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I113"/>
+  <dimension ref="A1:I102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.08984375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="17" style="2" customWidth="1"/>
-    <col min="3" max="3" width="54" style="2" customWidth="1"/>
+    <col min="1" max="1" width="19.453125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="23.81640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="74.1796875" style="2" customWidth="1"/>
     <col min="4" max="4" width="21.26953125" style="2" customWidth="1"/>
     <col min="5" max="5" width="20.7265625" style="2" customWidth="1"/>
     <col min="6" max="6" width="22.26953125" style="2" customWidth="1"/>
@@ -952,7 +977,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>110</v>
+        <v>82</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -961,10 +986,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>112</v>
+        <v>84</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -979,448 +1004,452 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="7"/>
       <c r="B3" s="3" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="7"/>
       <c r="B4" s="3" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="7"/>
       <c r="B5" s="3" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="7"/>
       <c r="B6" s="3" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="7"/>
       <c r="B7" s="3" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="7"/>
       <c r="B8" s="3" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="7"/>
       <c r="B9" s="3" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="7"/>
       <c r="B10" s="3" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="7"/>
       <c r="B11" s="3" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="7"/>
       <c r="B12" s="3" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="7"/>
       <c r="B13" s="3" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="8"/>
       <c r="B14" s="3" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>19</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>21</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="10"/>
       <c r="B16" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>22</v>
+        <v>160</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="10"/>
       <c r="B17" s="3" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>23</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="11"/>
       <c r="B18" s="3" t="s">
-        <v>41</v>
+        <v>161</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
         <v>42</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="10"/>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="11"/>
       <c r="B20" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="11"/>
+        <v>158</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="9" t="s">
+        <v>102</v>
+      </c>
       <c r="B21" s="3" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>45</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A22" s="9" t="s">
-        <v>53</v>
-      </c>
+      <c r="A22" s="11"/>
       <c r="B22" s="3" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>49</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A23" s="10"/>
+      <c r="A23" s="9" t="s">
+        <v>65</v>
+      </c>
       <c r="B23" s="3" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>50</v>
+        <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="10"/>
       <c r="B24" s="3" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>51</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A25" s="11"/>
+      <c r="A25" s="10"/>
       <c r="B25" s="3" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" s="9" t="s">
-        <v>58</v>
-      </c>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A26" s="10"/>
       <c r="B26" s="3" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="11"/>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A27" s="10"/>
       <c r="B27" s="3" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>60</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="9" t="s">
-        <v>65</v>
-      </c>
+      <c r="A28" s="10"/>
       <c r="B28" s="3" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>61</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A29" s="10"/>
+      <c r="A29" s="11"/>
       <c r="B29" s="3" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A30" s="10"/>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="12" t="s">
+        <v>135</v>
+      </c>
       <c r="B30" s="3" t="s">
-        <v>70</v>
+        <v>136</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A31" s="11"/>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="12" t="s">
+        <v>137</v>
+      </c>
       <c r="B31" s="3" t="s">
-        <v>71</v>
+        <v>138</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A32" s="9" t="s">
-        <v>74</v>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="12" t="s">
+        <v>139</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>80</v>
+        <v>140</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="11"/>
+        <v>155</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="34" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="12" t="s">
+        <v>141</v>
+      </c>
       <c r="B33" s="3" t="s">
-        <v>81</v>
+        <v>142</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A34" s="9" t="s">
-        <v>79</v>
+        <v>156</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="12" t="s">
+        <v>111</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>82</v>
+        <v>112</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A35" s="10"/>
+        <v>154</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="37" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="12" t="s">
+        <v>113</v>
+      </c>
       <c r="B35" s="3" t="s">
-        <v>83</v>
+        <v>114</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A36" s="10"/>
+        <v>153</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="12" t="s">
+        <v>115</v>
+      </c>
       <c r="B36" s="3" t="s">
-        <v>84</v>
+        <v>116</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A37" s="11"/>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="34" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="12" t="s">
+        <v>117</v>
+      </c>
       <c r="B37" s="3" t="s">
-        <v>85</v>
+        <v>118</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="9" t="s">
-        <v>86</v>
+        <v>151</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="12" t="s">
+        <v>119</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>99</v>
+        <v>121</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A39" s="10"/>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="12" t="s">
+        <v>120</v>
+      </c>
       <c r="B39" s="3" t="s">
-        <v>100</v>
+        <v>122</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="10"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="12" t="s">
+        <v>123</v>
+      </c>
       <c r="B40" s="3" t="s">
-        <v>101</v>
+        <v>124</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A41" s="10"/>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="12" t="s">
+        <v>125</v>
+      </c>
       <c r="B41" s="3" t="s">
-        <v>102</v>
+        <v>126</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A42" s="10"/>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="12" t="s">
+        <v>127</v>
+      </c>
       <c r="B42" s="3" t="s">
-        <v>103</v>
+        <v>128</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A43" s="10"/>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="31" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="12" t="s">
+        <v>129</v>
+      </c>
       <c r="B43" s="3" t="s">
-        <v>104</v>
+        <v>130</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A44" s="11"/>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="12" t="s">
+        <v>131</v>
+      </c>
       <c r="B44" s="3" t="s">
-        <v>105</v>
+        <v>132</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A45" s="9" t="s">
-        <v>98</v>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="12" t="s">
+        <v>133</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>106</v>
+        <v>134</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A46" s="10"/>
-      <c r="B46" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A47" s="10"/>
-      <c r="B47" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A48" s="11"/>
-      <c r="B48" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>97</v>
-      </c>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B46" s="3"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B47" s="3"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B48" s="3"/>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B49" s="3"/>
@@ -1584,51 +1613,13 @@
     <row r="102" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B102" s="3"/>
     </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B103" s="3"/>
-    </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B104" s="3"/>
-    </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B105" s="3"/>
-    </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B106" s="3"/>
-    </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B107" s="3"/>
-    </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B108" s="3"/>
-    </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B109" s="3"/>
-    </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B110" s="3"/>
-    </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B111" s="3"/>
-    </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B112" s="3"/>
-    </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B113" s="3"/>
-    </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="5">
     <mergeCell ref="A2:A14"/>
+    <mergeCell ref="A23:A29"/>
     <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="A38:A44"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -1637,12 +1628,217 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A3:C26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:C26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.90625" customWidth="1"/>
+    <col min="2" max="2" width="17.81640625" customWidth="1"/>
+    <col min="3" max="3" width="43.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="10"/>
+      <c r="B4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="10"/>
+      <c r="B5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="11"/>
+      <c r="B6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="10"/>
+      <c r="B9" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="10"/>
+      <c r="B10" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="11"/>
+      <c r="B11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="10"/>
+      <c r="B14" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" s="10"/>
+      <c r="B15" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="11"/>
+      <c r="B16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A18" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A19" s="10"/>
+      <c r="B19" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="10"/>
+      <c r="B20" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A21" s="11"/>
+      <c r="B21" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A23" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A24" s="10"/>
+      <c r="B24" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A25" s="10"/>
+      <c r="B25" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A26" s="11"/>
+      <c r="B26" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="A23:A26"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
enhanced verifying URL function; added Test_Cases
</commit_message>
<xml_diff>
--- a/ToTaL Test Cases.xlsx
+++ b/ToTaL Test Cases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="19420" windowHeight="9030"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="19420" windowHeight="9030" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="167">
   <si>
     <t>Test Cases</t>
   </si>
@@ -502,6 +502,21 @@
   </si>
   <si>
     <t>areaPos_tc_004</t>
+  </si>
+  <si>
+    <t>ERROR: parameter does not exist</t>
+  </si>
+  <si>
+    <t>Verify if a non-existing parameter is set, then API will return an error message.</t>
+  </si>
+  <si>
+    <t>unknownParameter</t>
+  </si>
+  <si>
+    <t>unknownParameter_tc_001</t>
+  </si>
+  <si>
+    <t>is it ERROR: if the value of non-required is empty?</t>
   </si>
 </sst>
 </file>
@@ -617,7 +632,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -633,6 +648,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -652,8 +673,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -956,16 +980,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I102"/>
+  <dimension ref="A1:I123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView topLeftCell="A61" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19.453125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="23.81640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="27.7265625" style="2" customWidth="1"/>
     <col min="3" max="3" width="74.1796875" style="2" customWidth="1"/>
     <col min="4" max="4" width="21.26953125" style="2" customWidth="1"/>
     <col min="5" max="5" width="20.7265625" style="2" customWidth="1"/>
@@ -1005,7 +1029,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1016,7 +1040,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="7"/>
+      <c r="A3" s="9"/>
       <c r="B3" s="3" t="s">
         <v>13</v>
       </c>
@@ -1025,7 +1049,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="7"/>
+      <c r="A4" s="9"/>
       <c r="B4" s="3" t="s">
         <v>14</v>
       </c>
@@ -1034,7 +1058,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="7"/>
+      <c r="A5" s="9"/>
       <c r="B5" s="3" t="s">
         <v>15</v>
       </c>
@@ -1043,7 +1067,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="7"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="3" t="s">
         <v>16</v>
       </c>
@@ -1052,7 +1076,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="7"/>
+      <c r="A7" s="9"/>
       <c r="B7" s="3" t="s">
         <v>17</v>
       </c>
@@ -1061,7 +1085,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="7"/>
+      <c r="A8" s="9"/>
       <c r="B8" s="3" t="s">
         <v>18</v>
       </c>
@@ -1070,7 +1094,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="7"/>
+      <c r="A9" s="9"/>
       <c r="B9" s="3" t="s">
         <v>19</v>
       </c>
@@ -1079,7 +1103,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="7"/>
+      <c r="A10" s="9"/>
       <c r="B10" s="3" t="s">
         <v>20</v>
       </c>
@@ -1088,7 +1112,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="7"/>
+      <c r="A11" s="9"/>
       <c r="B11" s="3" t="s">
         <v>21</v>
       </c>
@@ -1097,7 +1121,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="7"/>
+      <c r="A12" s="9"/>
       <c r="B12" s="3" t="s">
         <v>22</v>
       </c>
@@ -1106,7 +1130,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="7"/>
+      <c r="A13" s="9"/>
       <c r="B13" s="3" t="s">
         <v>23</v>
       </c>
@@ -1115,7 +1139,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="8"/>
+      <c r="A14" s="10"/>
       <c r="B14" s="3" t="s">
         <v>24</v>
       </c>
@@ -1123,428 +1147,567 @@
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="9" t="s">
+    <row r="15" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="12"/>
+      <c r="B16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" s="12"/>
+      <c r="B17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A18" s="13"/>
+      <c r="B18" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A19" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B19" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="10"/>
-      <c r="B16" s="3" t="s">
+    <row r="20" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="12"/>
+      <c r="B20" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A17" s="10"/>
-      <c r="B17" s="3" t="s">
+    <row r="21" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A21" s="12"/>
+      <c r="B21" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="11"/>
-      <c r="B18" s="3" t="s">
+    <row r="22" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A22" s="13"/>
+      <c r="B22" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="9" t="s">
+    <row r="23" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="12"/>
+      <c r="B24" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A25" s="12"/>
+      <c r="B25" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A26" s="13"/>
+      <c r="B26" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A27" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B27" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="11"/>
-      <c r="B20" s="3" t="s">
+    <row r="28" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A28" s="13"/>
+      <c r="B28" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="9" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A30" s="12"/>
+      <c r="B30" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A31" s="12"/>
+      <c r="B31" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A32" s="13"/>
+      <c r="B32" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B33" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A22" s="11"/>
-      <c r="B22" s="3" t="s">
+    <row r="34" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A34" s="13"/>
+      <c r="B34" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A23" s="9" t="s">
+    <row r="35" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="12"/>
+      <c r="B36" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A37" s="12"/>
+      <c r="B37" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A38" s="13"/>
+      <c r="B38" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A39" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B39" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C39" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24" s="10"/>
-      <c r="B24" s="3" t="s">
+    <row r="40" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A40" s="12"/>
+      <c r="B40" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C40" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A25" s="10"/>
-      <c r="B25" s="3" t="s">
+    <row r="41" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A41" s="12"/>
+      <c r="B41" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C41" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="10"/>
-      <c r="B26" s="3" t="s">
+    <row r="42" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A42" s="12"/>
+      <c r="B42" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C42" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A27" s="10"/>
-      <c r="B27" s="3" t="s">
+    <row r="43" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A43" s="12"/>
+      <c r="B43" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C43" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="10"/>
-      <c r="B28" s="3" t="s">
+    <row r="44" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A44" s="12"/>
+      <c r="B44" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C44" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A29" s="11"/>
-      <c r="B29" s="3" t="s">
+    <row r="45" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A45" s="13"/>
+      <c r="B45" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C45" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="12" t="s">
+    <row r="46" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="12"/>
+      <c r="B47" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A48" s="12"/>
+      <c r="B48" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A49" s="13"/>
+      <c r="B49" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" s="6"/>
+      <c r="B50" s="3"/>
+    </row>
+    <row r="51" spans="1:3" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B51" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C51" s="2" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="12" t="s">
+    <row r="52" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B52" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C52" s="2" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="12" t="s">
+    <row r="53" spans="1:3" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B53" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C53" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="34" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="12" t="s">
+    <row r="54" spans="1:3" ht="34" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B54" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C54" s="2" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="12" t="s">
+    <row r="55" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B55" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C55" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="37" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="12" t="s">
+    <row r="56" spans="1:3" ht="37" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B56" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C56" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="12" t="s">
+    <row r="57" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B57" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C57" s="2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="34" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="12" t="s">
+    <row r="58" spans="1:3" ht="34" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B58" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C58" s="2" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="12" t="s">
+    <row r="59" spans="1:3" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B59" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C59" s="2" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="12" t="s">
+    <row r="60" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B60" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C60" s="2" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="12" t="s">
+    <row r="61" spans="1:3" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B61" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C61" s="2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="12" t="s">
+    <row r="62" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B62" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C62" s="2" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="12" t="s">
+    <row r="63" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B63" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C63" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="12" t="s">
+    <row r="64" spans="1:3" ht="31" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B64" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C64" s="2" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="12" t="s">
+    <row r="65" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B65" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C65" s="2" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="12" t="s">
+    <row r="66" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B66" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C66" s="2" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B46" s="3"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B47" s="3"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B48" s="3"/>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B49" s="3"/>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B50" s="3"/>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B51" s="3"/>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B52" s="3"/>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B53" s="3"/>
-    </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B54" s="3"/>
-    </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B55" s="3"/>
-    </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B56" s="3"/>
-    </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B57" s="3"/>
-    </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B58" s="3"/>
-    </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B59" s="3"/>
-    </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B60" s="3"/>
-    </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B61" s="3"/>
-    </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B62" s="3"/>
-    </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B63" s="3"/>
-    </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B64" s="3"/>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B65" s="3"/>
-    </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B66" s="3"/>
-    </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B67" s="3"/>
-    </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" ht="34" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B68" s="3"/>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B69" s="3"/>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B70" s="3"/>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B71" s="3"/>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B72" s="3"/>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B73" s="3"/>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B74" s="3"/>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B75" s="3"/>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B76" s="3"/>
     </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B77" s="3"/>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B78" s="3"/>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B79" s="3"/>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B80" s="3"/>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.35">
@@ -1613,13 +1776,81 @@
     <row r="102" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B102" s="3"/>
     </row>
+    <row r="103" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B103" s="3"/>
+    </row>
+    <row r="104" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B104" s="3"/>
+    </row>
+    <row r="105" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B105" s="3"/>
+    </row>
+    <row r="106" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B106" s="3"/>
+    </row>
+    <row r="107" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B107" s="3"/>
+    </row>
+    <row r="108" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B108" s="3"/>
+    </row>
+    <row r="109" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B109" s="3"/>
+    </row>
+    <row r="110" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B110" s="3"/>
+    </row>
+    <row r="111" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B111" s="3"/>
+    </row>
+    <row r="112" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B112" s="3"/>
+    </row>
+    <row r="113" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B113" s="3"/>
+    </row>
+    <row r="114" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B114" s="3"/>
+    </row>
+    <row r="115" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B115" s="3"/>
+    </row>
+    <row r="116" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B116" s="3"/>
+    </row>
+    <row r="117" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B117" s="3"/>
+    </row>
+    <row r="118" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B118" s="3"/>
+    </row>
+    <row r="119" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B119" s="3"/>
+    </row>
+    <row r="120" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B120" s="3"/>
+    </row>
+    <row r="121" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B121" s="3"/>
+    </row>
+    <row r="122" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B122" s="3"/>
+    </row>
+    <row r="123" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B123" s="3"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="10">
+    <mergeCell ref="A46:A49"/>
     <mergeCell ref="A2:A14"/>
-    <mergeCell ref="A23:A29"/>
+    <mergeCell ref="A39:A45"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A33:A34"/>
     <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="A35:A38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -1628,10 +1859,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:C26"/>
+  <dimension ref="A3:C30"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:C26"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1642,7 +1873,7 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1653,7 +1884,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="10"/>
+      <c r="A4" s="12"/>
       <c r="B4" s="3" t="s">
         <v>26</v>
       </c>
@@ -1662,7 +1893,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="10"/>
+      <c r="A5" s="12"/>
       <c r="B5" s="3" t="s">
         <v>27</v>
       </c>
@@ -1671,7 +1902,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="11"/>
+      <c r="A6" s="13"/>
       <c r="B6" s="3" t="s">
         <v>28</v>
       </c>
@@ -1680,7 +1911,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="11" t="s">
         <v>37</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -1691,7 +1922,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="10"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="3" t="s">
         <v>39</v>
       </c>
@@ -1700,7 +1931,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="10"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="3" t="s">
         <v>40</v>
       </c>
@@ -1709,7 +1940,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="11"/>
+      <c r="A11" s="13"/>
       <c r="B11" s="3" t="s">
         <v>41</v>
       </c>
@@ -1718,7 +1949,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="11" t="s">
         <v>47</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -1729,7 +1960,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="10"/>
+      <c r="A14" s="12"/>
       <c r="B14" s="3" t="s">
         <v>51</v>
       </c>
@@ -1738,7 +1969,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="10"/>
+      <c r="A15" s="12"/>
       <c r="B15" s="3" t="s">
         <v>52</v>
       </c>
@@ -1747,7 +1978,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="11"/>
+      <c r="A16" s="13"/>
       <c r="B16" s="3" t="s">
         <v>53</v>
       </c>
@@ -1756,7 +1987,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="11" t="s">
         <v>58</v>
       </c>
       <c r="B18" s="3" t="s">
@@ -1767,7 +1998,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="10"/>
+      <c r="A19" s="12"/>
       <c r="B19" s="3" t="s">
         <v>62</v>
       </c>
@@ -1776,7 +2007,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="10"/>
+      <c r="A20" s="12"/>
       <c r="B20" s="3" t="s">
         <v>63</v>
       </c>
@@ -1785,7 +2016,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="11"/>
+      <c r="A21" s="13"/>
       <c r="B21" s="3" t="s">
         <v>64</v>
       </c>
@@ -1794,7 +2025,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="11" t="s">
         <v>70</v>
       </c>
       <c r="B23" s="3" t="s">
@@ -1805,7 +2036,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24" s="10"/>
+      <c r="A24" s="12"/>
       <c r="B24" s="3" t="s">
         <v>79</v>
       </c>
@@ -1814,7 +2045,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A25" s="10"/>
+      <c r="A25" s="12"/>
       <c r="B25" s="3" t="s">
         <v>80</v>
       </c>
@@ -1823,7 +2054,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="11"/>
+      <c r="A26" s="13"/>
       <c r="B26" s="3" t="s">
         <v>81</v>
       </c>
@@ -1831,8 +2062,24 @@
         <v>69</v>
       </c>
     </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A30:C30"/>
     <mergeCell ref="A3:A6"/>
     <mergeCell ref="A8:A11"/>
     <mergeCell ref="A13:A16"/>

</xml_diff>

<commit_message>
enhanced calculation of combination
</commit_message>
<xml_diff>
--- a/ToTaL Test Cases.xlsx
+++ b/ToTaL Test Cases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="19420" windowHeight="9030" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="19420" windowHeight="9030"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -649,11 +649,17 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -664,20 +670,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -980,10 +980,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I123"/>
+  <dimension ref="A1:I122"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1029,7 +1029,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1038,117 +1038,195 @@
       <c r="C2" s="2" t="s">
         <v>85</v>
       </c>
+      <c r="D2" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E2" s="15">
+        <v>43980</v>
+      </c>
     </row>
     <row r="3" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="9"/>
+      <c r="A3" s="11"/>
       <c r="B3" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>86</v>
       </c>
+      <c r="D3" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E3" s="15">
+        <v>43980</v>
+      </c>
     </row>
     <row r="4" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="9"/>
+      <c r="A4" s="11"/>
       <c r="B4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>87</v>
       </c>
+      <c r="D4" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E4" s="15">
+        <v>43980</v>
+      </c>
     </row>
     <row r="5" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="9"/>
+      <c r="A5" s="11"/>
       <c r="B5" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>88</v>
       </c>
+      <c r="D5" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E5" s="15">
+        <v>43980</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="9"/>
+      <c r="A6" s="11"/>
       <c r="B6" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>89</v>
       </c>
+      <c r="D6" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E6" s="15">
+        <v>43980</v>
+      </c>
     </row>
     <row r="7" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="9"/>
+      <c r="A7" s="11"/>
       <c r="B7" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>90</v>
       </c>
+      <c r="D7" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E7" s="15">
+        <v>43980</v>
+      </c>
     </row>
     <row r="8" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="9"/>
+      <c r="A8" s="11"/>
       <c r="B8" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>91</v>
       </c>
+      <c r="D8" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E8" s="15">
+        <v>43980</v>
+      </c>
     </row>
     <row r="9" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="9"/>
+      <c r="A9" s="11"/>
       <c r="B9" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>92</v>
       </c>
+      <c r="D9" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E9" s="15">
+        <v>43980</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="9"/>
+      <c r="A10" s="11"/>
       <c r="B10" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>93</v>
       </c>
+      <c r="D10" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E10" s="15">
+        <v>43980</v>
+      </c>
     </row>
     <row r="11" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="9"/>
+      <c r="A11" s="11"/>
       <c r="B11" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>94</v>
       </c>
+      <c r="D11" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E11" s="15">
+        <v>43980</v>
+      </c>
     </row>
     <row r="12" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="9"/>
+      <c r="A12" s="11"/>
       <c r="B12" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>95</v>
       </c>
+      <c r="D12" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E12" s="15">
+        <v>43980</v>
+      </c>
     </row>
     <row r="13" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="9"/>
+      <c r="A13" s="11"/>
       <c r="B13" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>96</v>
       </c>
+      <c r="D13" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E13" s="15">
+        <v>43980</v>
+      </c>
     </row>
     <row r="14" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="10"/>
+      <c r="A14" s="12"/>
       <c r="B14" s="3" t="s">
         <v>24</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>100</v>
       </c>
+      <c r="D14" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E14" s="15">
+        <v>43980</v>
+      </c>
     </row>
     <row r="15" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -1157,36 +1235,60 @@
       <c r="C15" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="D15" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E15" s="15">
+        <v>43980</v>
+      </c>
     </row>
     <row r="16" spans="1:9" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="12"/>
+      <c r="A16" s="8"/>
       <c r="B16" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A17" s="12"/>
+      <c r="D16" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E16" s="15">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" s="8"/>
       <c r="B17" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="13"/>
+      <c r="D17" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E17" s="15">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A18" s="9"/>
       <c r="B18" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="11" t="s">
+      <c r="D18" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E18" s="15">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A19" s="7" t="s">
         <v>29</v>
       </c>
       <c r="B19" s="3" t="s">
@@ -1195,36 +1297,60 @@
       <c r="C19" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="12"/>
+      <c r="D19" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E19" s="15">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="8"/>
       <c r="B20" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="12"/>
+      <c r="D20" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E20" s="15">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A21" s="8"/>
       <c r="B21" s="3" t="s">
         <v>32</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A22" s="13"/>
+      <c r="D21" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E21" s="15">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A22" s="9"/>
       <c r="B22" s="3" t="s">
         <v>161</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="11" t="s">
+      <c r="D22" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E22" s="15">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="7" t="s">
         <v>37</v>
       </c>
       <c r="B23" s="3" t="s">
@@ -1233,36 +1359,60 @@
       <c r="C23" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="12"/>
+      <c r="D23" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E23" s="15">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="8"/>
       <c r="B24" s="3" t="s">
         <v>39</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A25" s="12"/>
+      <c r="D24" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E24" s="15">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A25" s="8"/>
       <c r="B25" s="3" t="s">
         <v>40</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="13"/>
+      <c r="D25" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E25" s="15">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A26" s="9"/>
       <c r="B26" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A27" s="11" t="s">
+      <c r="D26" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E26" s="15">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A27" s="7" t="s">
         <v>42</v>
       </c>
       <c r="B27" s="3" t="s">
@@ -1271,18 +1421,30 @@
       <c r="C27" s="2" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="13"/>
+      <c r="D27" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E27" s="15">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A28" s="9"/>
       <c r="B28" s="3" t="s">
         <v>49</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" s="11" t="s">
+      <c r="D28" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E28" s="15">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" s="7" t="s">
         <v>47</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -1291,36 +1453,60 @@
       <c r="C29" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A30" s="12"/>
+      <c r="D29" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E29" s="15">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A30" s="8"/>
       <c r="B30" s="3" t="s">
         <v>51</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A31" s="12"/>
+      <c r="D30" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E30" s="15">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A31" s="8"/>
       <c r="B31" s="3" t="s">
         <v>52</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A32" s="13"/>
+      <c r="D31" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E31" s="15">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A32" s="9"/>
       <c r="B32" s="3" t="s">
         <v>53</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="11" t="s">
+      <c r="D32" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E32" s="15">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="7" t="s">
         <v>102</v>
       </c>
       <c r="B33" s="3" t="s">
@@ -1329,18 +1515,30 @@
       <c r="C33" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A34" s="13"/>
+      <c r="D33" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E33" s="15">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A34" s="9"/>
       <c r="B34" s="3" t="s">
         <v>60</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="11" t="s">
+      <c r="D34" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E34" s="15">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="7" t="s">
         <v>58</v>
       </c>
       <c r="B35" s="3" t="s">
@@ -1349,36 +1547,60 @@
       <c r="C35" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="12"/>
+      <c r="D35" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E35" s="15">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="8"/>
       <c r="B36" s="3" t="s">
         <v>62</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A37" s="12"/>
+      <c r="D36" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E36" s="15">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A37" s="8"/>
       <c r="B37" s="3" t="s">
         <v>63</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A38" s="13"/>
+      <c r="D37" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E37" s="15">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A38" s="9"/>
       <c r="B38" s="3" t="s">
         <v>64</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="11" t="s">
+      <c r="D38" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E38" s="15">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A39" s="7" t="s">
         <v>65</v>
       </c>
       <c r="B39" s="3" t="s">
@@ -1387,63 +1609,105 @@
       <c r="C39" s="2" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A40" s="12"/>
+      <c r="D39" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E39" s="15">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A40" s="8"/>
       <c r="B40" s="3" t="s">
         <v>72</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="12"/>
+      <c r="D40" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E40" s="15">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A41" s="8"/>
       <c r="B41" s="3" t="s">
         <v>73</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="12"/>
+      <c r="D41" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E41" s="15">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A42" s="8"/>
       <c r="B42" s="3" t="s">
         <v>74</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43" s="12"/>
+      <c r="D42" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E42" s="15">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A43" s="8"/>
       <c r="B43" s="3" t="s">
         <v>75</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="12"/>
+      <c r="D43" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E43" s="15">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A44" s="8"/>
       <c r="B44" s="3" t="s">
         <v>76</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A45" s="13"/>
+      <c r="D44" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E44" s="15">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A45" s="9"/>
       <c r="B45" s="3" t="s">
         <v>77</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="11" t="s">
+      <c r="D45" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E45" s="15">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="7" t="s">
         <v>70</v>
       </c>
       <c r="B46" s="3" t="s">
@@ -1452,262 +1716,387 @@
       <c r="C46" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="12"/>
+      <c r="D46" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E46" s="15">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="8"/>
       <c r="B47" s="3" t="s">
         <v>79</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A48" s="12"/>
+      <c r="D47" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E47" s="15">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A48" s="8"/>
       <c r="B48" s="3" t="s">
         <v>80</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A49" s="13"/>
+      <c r="D48" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E48" s="15">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A49" s="9"/>
       <c r="B49" s="3" t="s">
         <v>81</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A50" s="6"/>
-      <c r="B50" s="3"/>
-    </row>
-    <row r="51" spans="1:3" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="7" t="s">
+      <c r="D49" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E49" s="15">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="6" t="s">
         <v>135</v>
       </c>
+      <c r="B50" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D50" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E50" s="15">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="6" t="s">
+        <v>137</v>
+      </c>
       <c r="B51" s="3" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="7" t="s">
-        <v>137</v>
+      <c r="D51" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E51" s="15">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="6" t="s">
+        <v>139</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="7" t="s">
-        <v>139</v>
+        <v>155</v>
+      </c>
+      <c r="D52" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E52" s="15">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="6" t="s">
+        <v>141</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="34" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="7" t="s">
-        <v>141</v>
+        <v>156</v>
+      </c>
+      <c r="D53" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E53" s="15">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="6" t="s">
+        <v>111</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>142</v>
+        <v>112</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="7" t="s">
-        <v>111</v>
+        <v>154</v>
+      </c>
+      <c r="D54" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E54" s="15">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="37" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="6" t="s">
+        <v>113</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="37" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="7" t="s">
-        <v>113</v>
+        <v>153</v>
+      </c>
+      <c r="D55" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E55" s="15">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="6" t="s">
+        <v>115</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="7" t="s">
-        <v>115</v>
+        <v>152</v>
+      </c>
+      <c r="D56" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E56" s="15">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="6" t="s">
+        <v>117</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="34" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="7" t="s">
-        <v>117</v>
+        <v>151</v>
+      </c>
+      <c r="D57" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E57" s="15">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="6" t="s">
+        <v>119</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="7" t="s">
-        <v>119</v>
+        <v>149</v>
+      </c>
+      <c r="D58" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E58" s="15">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="6" t="s">
+        <v>120</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="7" t="s">
-        <v>120</v>
+        <v>150</v>
+      </c>
+      <c r="D59" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E59" s="15">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="6" t="s">
+        <v>123</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="7" t="s">
-        <v>123</v>
+        <v>143</v>
+      </c>
+      <c r="D60" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E60" s="15">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="6" t="s">
+        <v>125</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="7" t="s">
-        <v>125</v>
+        <v>144</v>
+      </c>
+      <c r="D61" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E61" s="15">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="6" t="s">
+        <v>127</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="7" t="s">
-        <v>127</v>
+        <v>145</v>
+      </c>
+      <c r="D62" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E62" s="15">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="31" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="6" t="s">
+        <v>129</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="7" t="s">
-        <v>129</v>
+        <v>146</v>
+      </c>
+      <c r="D63" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E63" s="15">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="6" t="s">
+        <v>131</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="7" t="s">
-        <v>131</v>
+        <v>147</v>
+      </c>
+      <c r="D64" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E64" s="15">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="6" t="s">
+        <v>133</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>134</v>
+        <v>148</v>
+      </c>
+      <c r="D65" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E65" s="15">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>165</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="34" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="C67" s="2" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D66" s="15">
+        <v>43980</v>
+      </c>
+      <c r="E66" s="15">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B67" s="3"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B68" s="3"/>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B69" s="3"/>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B70" s="3"/>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B71" s="3"/>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B72" s="3"/>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B73" s="3"/>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B74" s="3"/>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B75" s="3"/>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B76" s="3"/>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B77" s="3"/>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B78" s="3"/>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B79" s="3"/>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B80" s="3"/>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.35">
@@ -1835,9 +2224,6 @@
     </row>
     <row r="122" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B122" s="3"/>
-    </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B123" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -1861,8 +2247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:C30"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1873,7 +2259,7 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1884,7 +2270,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="12"/>
+      <c r="A4" s="8"/>
       <c r="B4" s="3" t="s">
         <v>26</v>
       </c>
@@ -1893,7 +2279,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="12"/>
+      <c r="A5" s="8"/>
       <c r="B5" s="3" t="s">
         <v>27</v>
       </c>
@@ -1902,7 +2288,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="13"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="3" t="s">
         <v>28</v>
       </c>
@@ -1911,7 +2297,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="7" t="s">
         <v>37</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -1922,7 +2308,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="12"/>
+      <c r="A9" s="8"/>
       <c r="B9" s="3" t="s">
         <v>39</v>
       </c>
@@ -1931,7 +2317,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="12"/>
+      <c r="A10" s="8"/>
       <c r="B10" s="3" t="s">
         <v>40</v>
       </c>
@@ -1940,7 +2326,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="13"/>
+      <c r="A11" s="9"/>
       <c r="B11" s="3" t="s">
         <v>41</v>
       </c>
@@ -1949,7 +2335,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="7" t="s">
         <v>47</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -1960,7 +2346,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="12"/>
+      <c r="A14" s="8"/>
       <c r="B14" s="3" t="s">
         <v>51</v>
       </c>
@@ -1969,7 +2355,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="12"/>
+      <c r="A15" s="8"/>
       <c r="B15" s="3" t="s">
         <v>52</v>
       </c>
@@ -1978,7 +2364,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="13"/>
+      <c r="A16" s="9"/>
       <c r="B16" s="3" t="s">
         <v>53</v>
       </c>
@@ -1987,7 +2373,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="7" t="s">
         <v>58</v>
       </c>
       <c r="B18" s="3" t="s">
@@ -1998,7 +2384,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="12"/>
+      <c r="A19" s="8"/>
       <c r="B19" s="3" t="s">
         <v>62</v>
       </c>
@@ -2007,7 +2393,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="12"/>
+      <c r="A20" s="8"/>
       <c r="B20" s="3" t="s">
         <v>63</v>
       </c>
@@ -2016,7 +2402,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="13"/>
+      <c r="A21" s="9"/>
       <c r="B21" s="3" t="s">
         <v>64</v>
       </c>
@@ -2025,7 +2411,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="7" t="s">
         <v>70</v>
       </c>
       <c r="B23" s="3" t="s">
@@ -2036,7 +2422,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24" s="12"/>
+      <c r="A24" s="8"/>
       <c r="B24" s="3" t="s">
         <v>79</v>
       </c>
@@ -2045,7 +2431,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A25" s="12"/>
+      <c r="A25" s="8"/>
       <c r="B25" s="3" t="s">
         <v>80</v>
       </c>
@@ -2054,7 +2440,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="13"/>
+      <c r="A26" s="9"/>
       <c r="B26" s="3" t="s">
         <v>81</v>
       </c>
@@ -2063,18 +2449,18 @@
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" s="14" t="s">
+      <c r="A28" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="13"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" s="15" t="s">
+      <c r="A30" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="B30" s="15"/>
-      <c r="C30" s="15"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
enhance combination calculation to be dynamic;added TC and enhanced URL validation
</commit_message>
<xml_diff>
--- a/ToTaL Test Cases.xlsx
+++ b/ToTaL Test Cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="258">
   <si>
     <t>Test Cases</t>
   </si>
@@ -306,9 +306,6 @@
     <t>Verify if groupBy parameter is set to CHIP, then API will return a tabular data based on the filter values applied.</t>
   </si>
   <si>
-    <t>Verify if groupBy parameter is set to FABLOT, then API will return a tabular data based on the filter values applied.</t>
-  </si>
-  <si>
     <t>Verify if area parameter is set to TEST, then API will return a tabular data based on the filter values applied.</t>
   </si>
   <si>
@@ -321,9 +318,6 @@
     <t>Verify if groupBy parameter is set to LOT, then API will return a tabular data based on the filter values applied.</t>
   </si>
   <si>
-    <t>Verify if time parameter is set to 1, then API will return a tabular data based on the filter values applied.</t>
-  </si>
-  <si>
     <t>local (positive)</t>
   </si>
   <si>
@@ -517,6 +511,285 @@
   </si>
   <si>
     <t>is it ERROR: if the value of non-required is empty?</t>
+  </si>
+  <si>
+    <t>tranDateNeg_tc_005</t>
+  </si>
+  <si>
+    <t>Verify if tranDate parameter is not set, then at least one of the non-required filter should be specified, otherwise it will return an error.</t>
+  </si>
+  <si>
+    <t>fabLocation (negative)</t>
+  </si>
+  <si>
+    <t>Verify if fabLocation parameter is set to a wild card, then API will return an error message.</t>
+  </si>
+  <si>
+    <t>Verify if fabLocation parameter is set to null then API will return an error message.</t>
+  </si>
+  <si>
+    <t>fabFacility (negative)</t>
+  </si>
+  <si>
+    <t>Verify if fabFacility parameter is set to a wild card, then API will return an error message.</t>
+  </si>
+  <si>
+    <t>Verify if fabFacility parameter is set to null then API will return an error message.</t>
+  </si>
+  <si>
+    <t>probeLocation (negative)</t>
+  </si>
+  <si>
+    <t>Verify if probeLocation parameter is set to a wild card, then API will return an error message.</t>
+  </si>
+  <si>
+    <t>Verify if probeLocation parameter is set to null then API will return an error message.</t>
+  </si>
+  <si>
+    <t>probeFacility (negative)</t>
+  </si>
+  <si>
+    <t>Verify if probeFacility parameter is set to a wild card, then API will return an error message.</t>
+  </si>
+  <si>
+    <t>Verify if probeFacility parameter is set to null then API will return an error message.</t>
+  </si>
+  <si>
+    <t>prtech (negative)</t>
+  </si>
+  <si>
+    <t>Verify if prtech parameter is set to a wild card, then API will return an error message.</t>
+  </si>
+  <si>
+    <t>Verify if prtech parameter is set to null then API will return an error message.</t>
+  </si>
+  <si>
+    <t>tech (negative)</t>
+  </si>
+  <si>
+    <t>Verify if tech parameter is set to a wild card, then API will return an error message.</t>
+  </si>
+  <si>
+    <t>Verify if tech parameter is set to null then API will return an error message.</t>
+  </si>
+  <si>
+    <t>ctech (negative)</t>
+  </si>
+  <si>
+    <t>Verify if tech ctech is set to a wild card, then API will return an error message.</t>
+  </si>
+  <si>
+    <t>Verify if tech ctech is set to null then API will return an error message.</t>
+  </si>
+  <si>
+    <t>sbe (negative)</t>
+  </si>
+  <si>
+    <t>Verify if sbe parameter is set to a wild card, then API will return an error message.</t>
+  </si>
+  <si>
+    <t>Verify if sbe parameter is set to null then API will return an error message.</t>
+  </si>
+  <si>
+    <t>sbe1 (negative)</t>
+  </si>
+  <si>
+    <t>Verify if sbe1 parameter is set to a wild card, then API will return an error message.</t>
+  </si>
+  <si>
+    <t>Verify if sbe1 parameter is set to null then API will return an error message.</t>
+  </si>
+  <si>
+    <t>sbe2 (negative)</t>
+  </si>
+  <si>
+    <t>Verify if sbe2 parameter is set to a wild card, then API will return an error message.</t>
+  </si>
+  <si>
+    <t>Verify if sbe2 parameter is set to null then API will return an error message.</t>
+  </si>
+  <si>
+    <t>device (negative)</t>
+  </si>
+  <si>
+    <t>Verify if device parameter is set to a wild card, then API will return an error message.</t>
+  </si>
+  <si>
+    <t>Verify if device parameter is set to null then API will return an error message.</t>
+  </si>
+  <si>
+    <t>material (negative)</t>
+  </si>
+  <si>
+    <t>Verify if material parameter is set to a wild card, then API will return an error message.</t>
+  </si>
+  <si>
+    <t>Verify if material parameter is set to null then API will return an error message.</t>
+  </si>
+  <si>
+    <t>chipname (negative)</t>
+  </si>
+  <si>
+    <t>Verify if chipname parameter is set to a wild card, then API will return an error message.</t>
+  </si>
+  <si>
+    <t>Verify if chipname parameter is set to null then API will return an error message.</t>
+  </si>
+  <si>
+    <t>fablot (negative)</t>
+  </si>
+  <si>
+    <t>Verify if fablot parameter is set to a wild card, then API will return an error message.</t>
+  </si>
+  <si>
+    <t>Verify if fablot parameter is set to null then API will return an error message.</t>
+  </si>
+  <si>
+    <t>lot (negative)</t>
+  </si>
+  <si>
+    <t>Verify if lot parameter is set to a wild card, then API will return an error message.</t>
+  </si>
+  <si>
+    <t>Verify if lot parameter is set to null then API will return an error message.</t>
+  </si>
+  <si>
+    <t>columns (negative)</t>
+  </si>
+  <si>
+    <t>Verify if columns parameter is set to a wild card, then API will return an error message.</t>
+  </si>
+  <si>
+    <t>Verify if columns parameter is set to null then API will return an error message.</t>
+  </si>
+  <si>
+    <t>Verify if columns parameter is set to String, then API will return an error message.</t>
+  </si>
+  <si>
+    <t>fabLocationNeg_tc_001</t>
+  </si>
+  <si>
+    <t>fabLocationNeg_tc_002</t>
+  </si>
+  <si>
+    <t>fabFacilityNeg_tc_001</t>
+  </si>
+  <si>
+    <t>fabFacilityNeg_tc_002</t>
+  </si>
+  <si>
+    <t>probeLocationNeg_tc_001</t>
+  </si>
+  <si>
+    <t>probeLocationNeg_tc_002</t>
+  </si>
+  <si>
+    <t>probeFacilityNeg_tc_001</t>
+  </si>
+  <si>
+    <t>probeFacilityNeg_tc_002</t>
+  </si>
+  <si>
+    <t>prtechNeg_tc_001</t>
+  </si>
+  <si>
+    <t>prtechNeg_tc_002</t>
+  </si>
+  <si>
+    <t>techNeg_tc_001</t>
+  </si>
+  <si>
+    <t>techNeg_tc_002</t>
+  </si>
+  <si>
+    <t>ctechNeg_tc_001</t>
+  </si>
+  <si>
+    <t>ctechNeg_tc_002</t>
+  </si>
+  <si>
+    <t>sbeNeg_tc_001</t>
+  </si>
+  <si>
+    <t>sbeNeg_tc_002</t>
+  </si>
+  <si>
+    <t>sbe1Neg_tc_001</t>
+  </si>
+  <si>
+    <t>sbe1Neg_tc_002</t>
+  </si>
+  <si>
+    <t>sbe2Neg_tc_001</t>
+  </si>
+  <si>
+    <t>sbe2Neg_tc_002</t>
+  </si>
+  <si>
+    <t>deviceNeg_tc_001</t>
+  </si>
+  <si>
+    <t>deviceNeg_tc_002</t>
+  </si>
+  <si>
+    <t>materialNeg_tc_001</t>
+  </si>
+  <si>
+    <t>materialNeg_tc_002</t>
+  </si>
+  <si>
+    <t>chipnameNeg_tc_001</t>
+  </si>
+  <si>
+    <t>chipnameNeg_tc_002</t>
+  </si>
+  <si>
+    <t>Verify if groupBy parameter is set to FAB, then API will return a tabular data based on the filter values applied.</t>
+  </si>
+  <si>
+    <t>local(negative)</t>
+  </si>
+  <si>
+    <t>Verify if time parameter is set to local, then API will return a tabular data based on the filter values applied.</t>
+  </si>
+  <si>
+    <t>fablotNeg_tc_001</t>
+  </si>
+  <si>
+    <t>fablotNeg_tc_002</t>
+  </si>
+  <si>
+    <t>lotNeg_tc_001</t>
+  </si>
+  <si>
+    <t>lotNeg_tc_002</t>
+  </si>
+  <si>
+    <t>columnsNeg_tc_001</t>
+  </si>
+  <si>
+    <t>columnsNeg_tc_002</t>
+  </si>
+  <si>
+    <t>columnsNeg_tc_003</t>
+  </si>
+  <si>
+    <t>columnsNeg_tc_004</t>
+  </si>
+  <si>
+    <t>Verify if columns parameter is set to non existing value allowed by specific area, then API will return an error message.</t>
+  </si>
+  <si>
+    <t>columnsNeg_tc_005</t>
+  </si>
+  <si>
+    <t>Verify if columns parameter is set to decimal value, then API will return an error message.</t>
+  </si>
+  <si>
+    <t>Verify if columns parameter is set to less than 0 value, then API will return an error message.</t>
+  </si>
+  <si>
+    <t>columnsNeg_tc_006</t>
   </si>
 </sst>
 </file>
@@ -554,7 +827,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -564,6 +837,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -632,7 +917,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -652,14 +937,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -670,14 +955,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -980,10 +1271,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I122"/>
+  <dimension ref="A1:I159"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1038,11 +1329,11 @@
       <c r="C2" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D2" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E2" s="15">
-        <v>43980</v>
+      <c r="D2" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E2" s="8">
+        <v>43973</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="29" x14ac:dyDescent="0.35">
@@ -1053,11 +1344,11 @@
       <c r="C3" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D3" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E3" s="15">
-        <v>43980</v>
+      <c r="D3" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E3" s="8">
+        <v>43973</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="29" x14ac:dyDescent="0.35">
@@ -1068,11 +1359,11 @@
       <c r="C4" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D4" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E4" s="15">
-        <v>43980</v>
+      <c r="D4" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E4" s="8">
+        <v>43973</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="29" x14ac:dyDescent="0.35">
@@ -1083,11 +1374,11 @@
       <c r="C5" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D5" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E5" s="15">
-        <v>43980</v>
+      <c r="D5" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E5" s="8">
+        <v>43973</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="29" x14ac:dyDescent="0.35">
@@ -1098,11 +1389,11 @@
       <c r="C6" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D6" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E6" s="15">
-        <v>43980</v>
+      <c r="D6" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E6" s="8">
+        <v>43973</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="29" x14ac:dyDescent="0.35">
@@ -1113,11 +1404,11 @@
       <c r="C7" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D7" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E7" s="15">
-        <v>43980</v>
+      <c r="D7" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E7" s="8">
+        <v>43973</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="29" x14ac:dyDescent="0.35">
@@ -1128,11 +1419,11 @@
       <c r="C8" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D8" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E8" s="15">
-        <v>43980</v>
+      <c r="D8" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E8" s="8">
+        <v>43973</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="29" x14ac:dyDescent="0.35">
@@ -1143,11 +1434,11 @@
       <c r="C9" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D9" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E9" s="15">
-        <v>43980</v>
+      <c r="D9" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E9" s="8">
+        <v>43973</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="29" x14ac:dyDescent="0.35">
@@ -1158,11 +1449,11 @@
       <c r="C10" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D10" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E10" s="15">
-        <v>43980</v>
+      <c r="D10" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E10" s="8">
+        <v>43973</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="29" x14ac:dyDescent="0.35">
@@ -1173,11 +1464,11 @@
       <c r="C11" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D11" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E11" s="15">
-        <v>43980</v>
+      <c r="D11" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E11" s="8">
+        <v>43973</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="29" x14ac:dyDescent="0.35">
@@ -1188,11 +1479,11 @@
       <c r="C12" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D12" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E12" s="15">
-        <v>43980</v>
+      <c r="D12" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E12" s="8">
+        <v>43973</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="29" x14ac:dyDescent="0.35">
@@ -1201,13 +1492,13 @@
         <v>23</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D13" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E13" s="15">
-        <v>43980</v>
+        <v>242</v>
+      </c>
+      <c r="D13" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E13" s="8">
+        <v>43973</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="29" x14ac:dyDescent="0.35">
@@ -1216,17 +1507,17 @@
         <v>24</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D14" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E14" s="15">
-        <v>43980</v>
+        <v>99</v>
+      </c>
+      <c r="D14" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E14" s="8">
+        <v>43973</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="13" t="s">
         <v>7</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -1235,122 +1526,122 @@
       <c r="C15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E15" s="15">
-        <v>43980</v>
+      <c r="D15" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E15" s="8">
+        <v>43973</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="8"/>
+      <c r="A16" s="14"/>
       <c r="B16" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E16" s="15">
-        <v>43980</v>
+      <c r="D16" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E16" s="8">
+        <v>43973</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A17" s="8"/>
+      <c r="A17" s="14"/>
       <c r="B17" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E17" s="15">
-        <v>43980</v>
+      <c r="D17" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E17" s="8">
+        <v>43973</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="9"/>
+      <c r="A18" s="15"/>
       <c r="B18" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E18" s="15">
-        <v>43980</v>
+      <c r="D18" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E18" s="8">
+        <v>43973</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="13" t="s">
         <v>29</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D19" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E19" s="15">
-        <v>43980</v>
+        <v>96</v>
+      </c>
+      <c r="D19" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E19" s="8">
+        <v>43973</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="8"/>
+      <c r="A20" s="14"/>
       <c r="B20" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="D20" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E20" s="15">
-        <v>43980</v>
+        <v>158</v>
+      </c>
+      <c r="D20" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E20" s="8">
+        <v>43973</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="8"/>
+      <c r="A21" s="14"/>
       <c r="B21" s="3" t="s">
         <v>32</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D21" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E21" s="8">
+        <v>43973</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A22" s="15"/>
+      <c r="B22" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D21" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E21" s="15">
-        <v>43980</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A22" s="9"/>
-      <c r="B22" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D22" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E22" s="15">
-        <v>43980</v>
+      <c r="D22" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E22" s="8">
+        <v>43973</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="13" t="s">
         <v>37</v>
       </c>
       <c r="B23" s="3" t="s">
@@ -1359,92 +1650,92 @@
       <c r="C23" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E23" s="15">
-        <v>43980</v>
+      <c r="D23" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E23" s="8">
+        <v>43973</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="8"/>
+      <c r="A24" s="14"/>
       <c r="B24" s="3" t="s">
         <v>39</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D24" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E24" s="15">
-        <v>43980</v>
+      <c r="D24" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E24" s="8">
+        <v>43973</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A25" s="8"/>
+      <c r="A25" s="14"/>
       <c r="B25" s="3" t="s">
         <v>40</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D25" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E25" s="15">
-        <v>43980</v>
+      <c r="D25" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E25" s="8">
+        <v>43973</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="9"/>
+      <c r="A26" s="15"/>
       <c r="B26" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D26" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E26" s="15">
-        <v>43980</v>
+      <c r="D26" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E26" s="8">
+        <v>43973</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="13" t="s">
         <v>42</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>48</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="D27" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E27" s="15">
-        <v>43980</v>
+        <v>157</v>
+      </c>
+      <c r="D27" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E27" s="8">
+        <v>43973</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="9"/>
+      <c r="A28" s="15"/>
       <c r="B28" s="3" t="s">
         <v>49</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="D28" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E28" s="15">
-        <v>43980</v>
+        <v>156</v>
+      </c>
+      <c r="D28" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E28" s="8">
+        <v>43973</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="13" t="s">
         <v>47</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -1453,93 +1744,93 @@
       <c r="C29" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D29" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E29" s="15">
-        <v>43980</v>
+      <c r="D29" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E29" s="8">
+        <v>43973</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A30" s="8"/>
+      <c r="A30" s="14"/>
       <c r="B30" s="3" t="s">
         <v>51</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E30" s="15">
-        <v>43980</v>
+      <c r="D30" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E30" s="8">
+        <v>43973</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A31" s="8"/>
+      <c r="A31" s="14"/>
       <c r="B31" s="3" t="s">
         <v>52</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D31" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E31" s="15">
-        <v>43980</v>
+      <c r="D31" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E31" s="8">
+        <v>43973</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A32" s="9"/>
+      <c r="A32" s="15"/>
       <c r="B32" s="3" t="s">
         <v>53</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D32" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E32" s="15">
-        <v>43980</v>
+      <c r="D32" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E32" s="8">
+        <v>43973</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="7" t="s">
-        <v>102</v>
+      <c r="A33" s="13" t="s">
+        <v>100</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D33" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E33" s="15">
-        <v>43980</v>
+        <v>101</v>
+      </c>
+      <c r="D33" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E33" s="8">
+        <v>43973</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A34" s="9"/>
+      <c r="A34" s="15"/>
       <c r="B34" s="3" t="s">
         <v>60</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D34" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E34" s="15">
-        <v>43980</v>
+        <v>244</v>
+      </c>
+      <c r="D34" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E34" s="8">
+        <v>43973</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="7" t="s">
-        <v>58</v>
+      <c r="A35" s="13" t="s">
+        <v>243</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>61</v>
@@ -1547,167 +1838,167 @@
       <c r="C35" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D35" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E35" s="15">
-        <v>43980</v>
+      <c r="D35" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E35" s="8">
+        <v>43973</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="8"/>
+      <c r="A36" s="14"/>
       <c r="B36" s="3" t="s">
         <v>62</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D36" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E36" s="15">
-        <v>43980</v>
+      <c r="D36" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E36" s="8">
+        <v>43973</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A37" s="8"/>
+      <c r="A37" s="14"/>
       <c r="B37" s="3" t="s">
         <v>63</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D37" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E37" s="15">
-        <v>43980</v>
+      <c r="D37" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E37" s="8">
+        <v>43973</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A38" s="9"/>
+      <c r="A38" s="15"/>
       <c r="B38" s="3" t="s">
         <v>64</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D38" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E38" s="15">
-        <v>43980</v>
+      <c r="D38" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E38" s="8">
+        <v>43973</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="7" t="s">
+      <c r="A39" s="13" t="s">
         <v>65</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>71</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D39" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E39" s="15">
-        <v>43980</v>
+        <v>108</v>
+      </c>
+      <c r="D39" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E39" s="8">
+        <v>43973</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A40" s="8"/>
+      <c r="A40" s="14"/>
       <c r="B40" s="3" t="s">
         <v>72</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D40" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E40" s="15">
-        <v>43980</v>
+        <v>102</v>
+      </c>
+      <c r="D40" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E40" s="8">
+        <v>43973</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="8"/>
+      <c r="A41" s="14"/>
       <c r="B41" s="3" t="s">
         <v>73</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D41" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E41" s="15">
-        <v>43980</v>
+        <v>103</v>
+      </c>
+      <c r="D41" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E41" s="8">
+        <v>43973</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="8"/>
+      <c r="A42" s="14"/>
       <c r="B42" s="3" t="s">
         <v>74</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D42" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E42" s="15">
-        <v>43980</v>
+        <v>104</v>
+      </c>
+      <c r="D42" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E42" s="8">
+        <v>43973</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43" s="8"/>
+      <c r="A43" s="14"/>
       <c r="B43" s="3" t="s">
         <v>75</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="D43" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E43" s="15">
-        <v>43980</v>
+        <v>105</v>
+      </c>
+      <c r="D43" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E43" s="8">
+        <v>43973</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="8"/>
+      <c r="A44" s="14"/>
       <c r="B44" s="3" t="s">
         <v>76</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="D44" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E44" s="15">
-        <v>43980</v>
+        <v>106</v>
+      </c>
+      <c r="D44" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E44" s="8">
+        <v>43973</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A45" s="9"/>
+      <c r="A45" s="15"/>
       <c r="B45" s="3" t="s">
         <v>77</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D45" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E45" s="15">
-        <v>43980</v>
+        <v>107</v>
+      </c>
+      <c r="D45" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E45" s="8">
+        <v>43973</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="7" t="s">
+      <c r="A46" s="13" t="s">
         <v>70</v>
       </c>
       <c r="B46" s="3" t="s">
@@ -1716,483 +2007,999 @@
       <c r="C46" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D46" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E46" s="15">
-        <v>43980</v>
+      <c r="D46" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E46" s="8">
+        <v>43973</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="8"/>
+      <c r="A47" s="14"/>
       <c r="B47" s="3" t="s">
         <v>79</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D47" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E47" s="15">
-        <v>43980</v>
+      <c r="D47" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E47" s="8">
+        <v>43973</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A48" s="8"/>
+      <c r="A48" s="14"/>
       <c r="B48" s="3" t="s">
         <v>80</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D48" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E48" s="15">
-        <v>43980</v>
+      <c r="D48" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E48" s="8">
+        <v>43973</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A49" s="9"/>
+      <c r="A49" s="14"/>
       <c r="B49" s="3" t="s">
         <v>81</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D49" s="15">
+      <c r="D49" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E49" s="8">
+        <v>43973</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="15"/>
+      <c r="B50" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D50" s="9">
+        <v>43985</v>
+      </c>
+      <c r="E50" s="9">
+        <v>43985</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D51" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E51" s="8">
+        <v>43973</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D52" s="9">
+        <v>43986</v>
+      </c>
+      <c r="E52" s="9">
+        <v>43986</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="D53" s="9">
+        <v>43986</v>
+      </c>
+      <c r="E53" s="9">
+        <v>43986</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D54" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E54" s="8">
+        <v>43973</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D55" s="9">
+        <v>43986</v>
+      </c>
+      <c r="E55" s="9">
+        <v>43986</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D56" s="9">
+        <v>43986</v>
+      </c>
+      <c r="E56" s="9">
+        <v>43986</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D57" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E57" s="8">
+        <v>43973</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D58" s="9">
+        <v>43986</v>
+      </c>
+      <c r="E58" s="9">
+        <v>43986</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D59" s="9">
+        <v>43986</v>
+      </c>
+      <c r="E59" s="9">
+        <v>43986</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D60" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E60" s="8">
+        <v>43973</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D61" s="9">
+        <v>43986</v>
+      </c>
+      <c r="E61" s="9">
+        <v>43986</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D62" s="9">
+        <v>43986</v>
+      </c>
+      <c r="E62" s="9">
+        <v>43986</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D63" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E63" s="8">
+        <v>43973</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D64" s="9">
+        <v>43986</v>
+      </c>
+      <c r="E64" s="9">
+        <v>43986</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D65" s="9">
+        <v>43986</v>
+      </c>
+      <c r="E65" s="9">
+        <v>43986</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="37" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D66" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E66" s="8">
+        <v>43973</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="37" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D67" s="9">
+        <v>43986</v>
+      </c>
+      <c r="E67" s="9">
+        <v>43986</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="37" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D68" s="9">
+        <v>43986</v>
+      </c>
+      <c r="E68" s="9">
+        <v>43986</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D69" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E69" s="8">
+        <v>43973</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D70" s="9">
+        <v>43986</v>
+      </c>
+      <c r="E70" s="9">
+        <v>43986</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D71" s="9">
+        <v>43986</v>
+      </c>
+      <c r="E71" s="9">
+        <v>43986</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D72" s="7">
         <v>43980</v>
       </c>
-      <c r="E49" s="15">
+      <c r="E72" s="7">
         <v>43980</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="D50" s="15">
+    <row r="73" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D73" s="9">
+        <v>43986</v>
+      </c>
+      <c r="E73" s="9">
+        <v>43986</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D74" s="9">
+        <v>43986</v>
+      </c>
+      <c r="E74" s="9">
+        <v>43986</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D75" s="7">
         <v>43980</v>
       </c>
-      <c r="E50" s="15">
+      <c r="E75" s="7">
         <v>43980</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="D51" s="15">
+    <row r="76" spans="1:5" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D76" s="9">
+        <v>43986</v>
+      </c>
+      <c r="E76" s="9">
+        <v>43986</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D77" s="9">
+        <v>43986</v>
+      </c>
+      <c r="E77" s="9">
+        <v>43986</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D78" s="7">
         <v>43980</v>
       </c>
-      <c r="E51" s="15">
+      <c r="E78" s="7">
         <v>43980</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="D52" s="15">
+    <row r="79" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A79" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="D79" s="9">
+        <v>43986</v>
+      </c>
+      <c r="E79" s="9">
+        <v>43986</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A80" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D80" s="9">
+        <v>43986</v>
+      </c>
+      <c r="E80" s="9">
+        <v>43986</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D81" s="7">
         <v>43980</v>
       </c>
-      <c r="E52" s="15">
+      <c r="E81" s="7">
         <v>43980</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="B53" s="3" t="s">
+    <row r="82" spans="1:5" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A82" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D82" s="9">
+        <v>43986</v>
+      </c>
+      <c r="E82" s="9">
+        <v>43986</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A83" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D83" s="9">
+        <v>43986</v>
+      </c>
+      <c r="E83" s="9">
+        <v>43986</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A84" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C84" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C53" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="D53" s="15">
+      <c r="D84" s="7">
         <v>43980</v>
       </c>
-      <c r="E53" s="15">
+      <c r="E84" s="7">
         <v>43980</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="D54" s="15">
+    <row r="85" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A85" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D85" s="9">
+        <v>43986</v>
+      </c>
+      <c r="E85" s="9">
+        <v>43986</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A86" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D86" s="9">
+        <v>43986</v>
+      </c>
+      <c r="E86" s="9">
+        <v>43986</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A87" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D87" s="7">
         <v>43980</v>
       </c>
-      <c r="E54" s="15">
+      <c r="E87" s="7">
         <v>43980</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="37" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="D55" s="15">
+    <row r="88" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A88" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D88" s="9">
+        <v>43986</v>
+      </c>
+      <c r="E88" s="9">
+        <v>43986</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A89" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="D89" s="9">
+        <v>43986</v>
+      </c>
+      <c r="E89" s="9">
+        <v>43986</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="31" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A90" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D90" s="7">
         <v>43980</v>
       </c>
-      <c r="E55" s="15">
+      <c r="E90" s="7">
         <v>43980</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="D56" s="15">
+    <row r="91" spans="1:5" ht="31" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A91" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="D91" s="9">
+        <v>43986</v>
+      </c>
+      <c r="E91" s="9">
+        <v>43986</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="31" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A92" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D92" s="9">
+        <v>43986</v>
+      </c>
+      <c r="E92" s="9">
+        <v>43986</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A93" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D93" s="7">
         <v>43980</v>
       </c>
-      <c r="E56" s="15">
+      <c r="E93" s="7">
         <v>43980</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="D57" s="15">
+    <row r="94" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A94" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="D94" s="9">
+        <v>43986</v>
+      </c>
+      <c r="E94" s="9">
+        <v>43986</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A95" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="D95" s="9">
+        <v>43986</v>
+      </c>
+      <c r="E95" s="9">
+        <v>43986</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A96" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D96" s="7">
         <v>43980</v>
       </c>
-      <c r="E57" s="15">
+      <c r="E96" s="7">
         <v>43980</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="D58" s="15">
+    <row r="97" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A97" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="D97" s="9">
+        <v>43986</v>
+      </c>
+      <c r="E97" s="9">
+        <v>43986</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A98" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D98" s="9">
+        <v>43986</v>
+      </c>
+      <c r="E98" s="9">
+        <v>43986</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A99" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="D99" s="9">
+        <v>43986</v>
+      </c>
+      <c r="E99" s="9">
+        <v>43986</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="38" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A100" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="D100" s="9">
+        <v>43986</v>
+      </c>
+      <c r="E100" s="9">
+        <v>43986</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="38" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A101" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="D101" s="9">
+        <v>43986</v>
+      </c>
+      <c r="E101" s="9">
+        <v>43986</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="38" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A102" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="D102" s="9">
+        <v>43986</v>
+      </c>
+      <c r="E102" s="9">
+        <v>43986</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A103" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D103" s="7">
         <v>43980</v>
       </c>
-      <c r="E58" s="15">
+      <c r="E103" s="7">
         <v>43980</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D59" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E59" s="15">
-        <v>43980</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="D60" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E60" s="15">
-        <v>43980</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="D61" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E61" s="15">
-        <v>43980</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="D62" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E62" s="15">
-        <v>43980</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="D63" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E63" s="15">
-        <v>43980</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D64" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E64" s="15">
-        <v>43980</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="D65" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E65" s="15">
-        <v>43980</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="D66" s="15">
-        <v>43980</v>
-      </c>
-      <c r="E66" s="15">
-        <v>43980</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B67" s="3"/>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B68" s="3"/>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B69" s="3"/>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B70" s="3"/>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B71" s="3"/>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B72" s="3"/>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B73" s="3"/>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B74" s="3"/>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B75" s="3"/>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B76" s="3"/>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B77" s="3"/>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B78" s="3"/>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B79" s="3"/>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B80" s="3"/>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B81" s="3"/>
-    </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B82" s="3"/>
-    </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B83" s="3"/>
-    </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B84" s="3"/>
-    </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B85" s="3"/>
-    </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B86" s="3"/>
-    </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B87" s="3"/>
-    </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B88" s="3"/>
-    </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B89" s="3"/>
-    </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B90" s="3"/>
-    </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B91" s="3"/>
-    </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B92" s="3"/>
-    </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B93" s="3"/>
-    </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B94" s="3"/>
-    </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B95" s="3"/>
-    </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B96" s="3"/>
-    </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B97" s="3"/>
-    </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B98" s="3"/>
-    </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B99" s="3"/>
-    </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B100" s="3"/>
-    </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B101" s="3"/>
-    </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B102" s="3"/>
-    </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B103" s="3"/>
-    </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B104" s="3"/>
     </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B105" s="3"/>
     </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B106" s="3"/>
     </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B107" s="3"/>
     </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B108" s="3"/>
     </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B109" s="3"/>
     </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B110" s="3"/>
     </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B111" s="3"/>
     </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B112" s="3"/>
     </row>
     <row r="113" spans="2:2" x14ac:dyDescent="0.35">
@@ -2225,9 +3032,120 @@
     <row r="122" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B122" s="3"/>
     </row>
+    <row r="123" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B123" s="3"/>
+    </row>
+    <row r="124" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B124" s="3"/>
+    </row>
+    <row r="125" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B125" s="3"/>
+    </row>
+    <row r="126" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B126" s="3"/>
+    </row>
+    <row r="127" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B127" s="3"/>
+    </row>
+    <row r="128" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B128" s="3"/>
+    </row>
+    <row r="129" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B129" s="3"/>
+    </row>
+    <row r="130" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B130" s="3"/>
+    </row>
+    <row r="131" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B131" s="3"/>
+    </row>
+    <row r="132" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B132" s="3"/>
+    </row>
+    <row r="133" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B133" s="3"/>
+    </row>
+    <row r="134" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B134" s="3"/>
+    </row>
+    <row r="135" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B135" s="3"/>
+    </row>
+    <row r="136" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B136" s="3"/>
+    </row>
+    <row r="137" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B137" s="3"/>
+    </row>
+    <row r="138" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B138" s="3"/>
+    </row>
+    <row r="139" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B139" s="3"/>
+    </row>
+    <row r="140" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B140" s="3"/>
+    </row>
+    <row r="141" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B141" s="3"/>
+    </row>
+    <row r="142" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B142" s="3"/>
+    </row>
+    <row r="143" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B143" s="3"/>
+    </row>
+    <row r="144" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B144" s="3"/>
+    </row>
+    <row r="145" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B145" s="3"/>
+    </row>
+    <row r="146" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B146" s="3"/>
+    </row>
+    <row r="147" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B147" s="3"/>
+    </row>
+    <row r="148" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B148" s="3"/>
+    </row>
+    <row r="149" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B149" s="3"/>
+    </row>
+    <row r="150" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B150" s="3"/>
+    </row>
+    <row r="151" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B151" s="3"/>
+    </row>
+    <row r="152" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B152" s="3"/>
+    </row>
+    <row r="153" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B153" s="3"/>
+    </row>
+    <row r="154" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B154" s="3"/>
+    </row>
+    <row r="155" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B155" s="3"/>
+    </row>
+    <row r="156" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B156" s="3"/>
+    </row>
+    <row r="157" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B157" s="3"/>
+    </row>
+    <row r="158" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B158" s="3"/>
+    </row>
+    <row r="159" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B159" s="3"/>
+    </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="A46:A49"/>
+    <mergeCell ref="A46:A50"/>
     <mergeCell ref="A2:A14"/>
     <mergeCell ref="A39:A45"/>
     <mergeCell ref="A19:A22"/>
@@ -2259,7 +3177,7 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="13" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -2270,7 +3188,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="8"/>
+      <c r="A4" s="14"/>
       <c r="B4" s="3" t="s">
         <v>26</v>
       </c>
@@ -2279,7 +3197,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="8"/>
+      <c r="A5" s="14"/>
       <c r="B5" s="3" t="s">
         <v>27</v>
       </c>
@@ -2288,7 +3206,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="9"/>
+      <c r="A6" s="15"/>
       <c r="B6" s="3" t="s">
         <v>28</v>
       </c>
@@ -2297,7 +3215,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="13" t="s">
         <v>37</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -2308,7 +3226,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="8"/>
+      <c r="A9" s="14"/>
       <c r="B9" s="3" t="s">
         <v>39</v>
       </c>
@@ -2317,7 +3235,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="8"/>
+      <c r="A10" s="14"/>
       <c r="B10" s="3" t="s">
         <v>40</v>
       </c>
@@ -2326,7 +3244,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="9"/>
+      <c r="A11" s="15"/>
       <c r="B11" s="3" t="s">
         <v>41</v>
       </c>
@@ -2335,7 +3253,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="13" t="s">
         <v>47</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -2346,7 +3264,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="8"/>
+      <c r="A14" s="14"/>
       <c r="B14" s="3" t="s">
         <v>51</v>
       </c>
@@ -2355,7 +3273,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="8"/>
+      <c r="A15" s="14"/>
       <c r="B15" s="3" t="s">
         <v>52</v>
       </c>
@@ -2364,7 +3282,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="9"/>
+      <c r="A16" s="15"/>
       <c r="B16" s="3" t="s">
         <v>53</v>
       </c>
@@ -2373,7 +3291,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="13" t="s">
         <v>58</v>
       </c>
       <c r="B18" s="3" t="s">
@@ -2384,7 +3302,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="8"/>
+      <c r="A19" s="14"/>
       <c r="B19" s="3" t="s">
         <v>62</v>
       </c>
@@ -2393,7 +3311,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="8"/>
+      <c r="A20" s="14"/>
       <c r="B20" s="3" t="s">
         <v>63</v>
       </c>
@@ -2402,7 +3320,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="9"/>
+      <c r="A21" s="15"/>
       <c r="B21" s="3" t="s">
         <v>64</v>
       </c>
@@ -2411,7 +3329,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="13" t="s">
         <v>70</v>
       </c>
       <c r="B23" s="3" t="s">
@@ -2422,7 +3340,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24" s="8"/>
+      <c r="A24" s="14"/>
       <c r="B24" s="3" t="s">
         <v>79</v>
       </c>
@@ -2431,7 +3349,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A25" s="8"/>
+      <c r="A25" s="14"/>
       <c r="B25" s="3" t="s">
         <v>80</v>
       </c>
@@ -2440,7 +3358,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="9"/>
+      <c r="A26" s="15"/>
       <c r="B26" s="3" t="s">
         <v>81</v>
       </c>
@@ -2449,18 +3367,18 @@
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" s="13" t="s">
-        <v>166</v>
-      </c>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
+      <c r="A28" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
+      <c r="A30" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
removed unnecessary code; added -TC
</commit_message>
<xml_diff>
--- a/ToTaL Test Cases.xlsx
+++ b/ToTaL Test Cases.xlsx
@@ -827,7 +827,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -843,12 +843,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -917,7 +911,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -943,8 +937,14 @@
     <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -953,15 +953,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1273,8 +1264,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1320,7 +1311,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="12" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1337,7 +1328,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="11"/>
+      <c r="A3" s="13"/>
       <c r="B3" s="3" t="s">
         <v>13</v>
       </c>
@@ -1352,7 +1343,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="11"/>
+      <c r="A4" s="13"/>
       <c r="B4" s="3" t="s">
         <v>14</v>
       </c>
@@ -1367,7 +1358,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="11"/>
+      <c r="A5" s="13"/>
       <c r="B5" s="3" t="s">
         <v>15</v>
       </c>
@@ -1382,7 +1373,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="11"/>
+      <c r="A6" s="13"/>
       <c r="B6" s="3" t="s">
         <v>16</v>
       </c>
@@ -1397,7 +1388,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="11"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="3" t="s">
         <v>17</v>
       </c>
@@ -1412,7 +1403,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="11"/>
+      <c r="A8" s="13"/>
       <c r="B8" s="3" t="s">
         <v>18</v>
       </c>
@@ -1427,7 +1418,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="11"/>
+      <c r="A9" s="13"/>
       <c r="B9" s="3" t="s">
         <v>19</v>
       </c>
@@ -1442,7 +1433,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="11"/>
+      <c r="A10" s="13"/>
       <c r="B10" s="3" t="s">
         <v>20</v>
       </c>
@@ -1457,7 +1448,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="11"/>
+      <c r="A11" s="13"/>
       <c r="B11" s="3" t="s">
         <v>21</v>
       </c>
@@ -1472,7 +1463,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="11"/>
+      <c r="A12" s="13"/>
       <c r="B12" s="3" t="s">
         <v>22</v>
       </c>
@@ -1487,7 +1478,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="11"/>
+      <c r="A13" s="13"/>
       <c r="B13" s="3" t="s">
         <v>23</v>
       </c>
@@ -1502,7 +1493,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="12"/>
+      <c r="A14" s="14"/>
       <c r="B14" s="3" t="s">
         <v>24</v>
       </c>
@@ -1517,7 +1508,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="9" t="s">
         <v>7</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -1534,7 +1525,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="14"/>
+      <c r="A16" s="10"/>
       <c r="B16" s="3" t="s">
         <v>26</v>
       </c>
@@ -1549,7 +1540,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A17" s="14"/>
+      <c r="A17" s="10"/>
       <c r="B17" s="3" t="s">
         <v>27</v>
       </c>
@@ -1564,7 +1555,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="15"/>
+      <c r="A18" s="11"/>
       <c r="B18" s="3" t="s">
         <v>28</v>
       </c>
@@ -1579,7 +1570,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="9" t="s">
         <v>29</v>
       </c>
       <c r="B19" s="3" t="s">
@@ -1596,7 +1587,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="14"/>
+      <c r="A20" s="10"/>
       <c r="B20" s="3" t="s">
         <v>31</v>
       </c>
@@ -1611,7 +1602,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="14"/>
+      <c r="A21" s="10"/>
       <c r="B21" s="3" t="s">
         <v>32</v>
       </c>
@@ -1626,7 +1617,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A22" s="15"/>
+      <c r="A22" s="11"/>
       <c r="B22" s="3" t="s">
         <v>159</v>
       </c>
@@ -1641,7 +1632,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="9" t="s">
         <v>37</v>
       </c>
       <c r="B23" s="3" t="s">
@@ -1658,7 +1649,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="14"/>
+      <c r="A24" s="10"/>
       <c r="B24" s="3" t="s">
         <v>39</v>
       </c>
@@ -1673,7 +1664,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A25" s="14"/>
+      <c r="A25" s="10"/>
       <c r="B25" s="3" t="s">
         <v>40</v>
       </c>
@@ -1688,7 +1679,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="15"/>
+      <c r="A26" s="11"/>
       <c r="B26" s="3" t="s">
         <v>41</v>
       </c>
@@ -1703,7 +1694,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A27" s="13" t="s">
+      <c r="A27" s="9" t="s">
         <v>42</v>
       </c>
       <c r="B27" s="3" t="s">
@@ -1720,7 +1711,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="15"/>
+      <c r="A28" s="11"/>
       <c r="B28" s="3" t="s">
         <v>49</v>
       </c>
@@ -1735,7 +1726,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="13" t="s">
+      <c r="A29" s="9" t="s">
         <v>47</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -1752,7 +1743,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A30" s="14"/>
+      <c r="A30" s="10"/>
       <c r="B30" s="3" t="s">
         <v>51</v>
       </c>
@@ -1767,7 +1758,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A31" s="14"/>
+      <c r="A31" s="10"/>
       <c r="B31" s="3" t="s">
         <v>52</v>
       </c>
@@ -1782,7 +1773,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A32" s="15"/>
+      <c r="A32" s="11"/>
       <c r="B32" s="3" t="s">
         <v>53</v>
       </c>
@@ -1797,7 +1788,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="13" t="s">
+      <c r="A33" s="9" t="s">
         <v>100</v>
       </c>
       <c r="B33" s="3" t="s">
@@ -1814,7 +1805,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A34" s="15"/>
+      <c r="A34" s="11"/>
       <c r="B34" s="3" t="s">
         <v>60</v>
       </c>
@@ -1829,7 +1820,7 @@
       </c>
     </row>
     <row r="35" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="13" t="s">
+      <c r="A35" s="9" t="s">
         <v>243</v>
       </c>
       <c r="B35" s="3" t="s">
@@ -1846,7 +1837,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="14"/>
+      <c r="A36" s="10"/>
       <c r="B36" s="3" t="s">
         <v>62</v>
       </c>
@@ -1861,7 +1852,7 @@
       </c>
     </row>
     <row r="37" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A37" s="14"/>
+      <c r="A37" s="10"/>
       <c r="B37" s="3" t="s">
         <v>63</v>
       </c>
@@ -1876,7 +1867,7 @@
       </c>
     </row>
     <row r="38" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A38" s="15"/>
+      <c r="A38" s="11"/>
       <c r="B38" s="3" t="s">
         <v>64</v>
       </c>
@@ -1891,7 +1882,7 @@
       </c>
     </row>
     <row r="39" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="13" t="s">
+      <c r="A39" s="9" t="s">
         <v>65</v>
       </c>
       <c r="B39" s="3" t="s">
@@ -1908,7 +1899,7 @@
       </c>
     </row>
     <row r="40" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A40" s="14"/>
+      <c r="A40" s="10"/>
       <c r="B40" s="3" t="s">
         <v>72</v>
       </c>
@@ -1923,7 +1914,7 @@
       </c>
     </row>
     <row r="41" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="14"/>
+      <c r="A41" s="10"/>
       <c r="B41" s="3" t="s">
         <v>73</v>
       </c>
@@ -1938,7 +1929,7 @@
       </c>
     </row>
     <row r="42" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="14"/>
+      <c r="A42" s="10"/>
       <c r="B42" s="3" t="s">
         <v>74</v>
       </c>
@@ -1953,7 +1944,7 @@
       </c>
     </row>
     <row r="43" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43" s="14"/>
+      <c r="A43" s="10"/>
       <c r="B43" s="3" t="s">
         <v>75</v>
       </c>
@@ -1968,7 +1959,7 @@
       </c>
     </row>
     <row r="44" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="14"/>
+      <c r="A44" s="10"/>
       <c r="B44" s="3" t="s">
         <v>76</v>
       </c>
@@ -1983,7 +1974,7 @@
       </c>
     </row>
     <row r="45" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A45" s="15"/>
+      <c r="A45" s="11"/>
       <c r="B45" s="3" t="s">
         <v>77</v>
       </c>
@@ -1998,7 +1989,7 @@
       </c>
     </row>
     <row r="46" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="13" t="s">
+      <c r="A46" s="9" t="s">
         <v>70</v>
       </c>
       <c r="B46" s="3" t="s">
@@ -2015,7 +2006,7 @@
       </c>
     </row>
     <row r="47" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="14"/>
+      <c r="A47" s="10"/>
       <c r="B47" s="3" t="s">
         <v>79</v>
       </c>
@@ -2030,7 +2021,7 @@
       </c>
     </row>
     <row r="48" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A48" s="14"/>
+      <c r="A48" s="10"/>
       <c r="B48" s="3" t="s">
         <v>80</v>
       </c>
@@ -2045,7 +2036,7 @@
       </c>
     </row>
     <row r="49" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A49" s="14"/>
+      <c r="A49" s="10"/>
       <c r="B49" s="3" t="s">
         <v>81</v>
       </c>
@@ -2060,17 +2051,17 @@
       </c>
     </row>
     <row r="50" spans="1:5" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="15"/>
+      <c r="A50" s="11"/>
       <c r="B50" s="3" t="s">
         <v>165</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="D50" s="9">
+      <c r="D50" s="8">
         <v>43985</v>
       </c>
-      <c r="E50" s="9">
+      <c r="E50" s="8">
         <v>43985</v>
       </c>
     </row>
@@ -2101,10 +2092,10 @@
       <c r="C52" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="D52" s="9">
-        <v>43986</v>
-      </c>
-      <c r="E52" s="9">
+      <c r="D52" s="8">
+        <v>43986</v>
+      </c>
+      <c r="E52" s="8">
         <v>43986</v>
       </c>
     </row>
@@ -2118,10 +2109,10 @@
       <c r="C53" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="D53" s="9">
-        <v>43986</v>
-      </c>
-      <c r="E53" s="9">
+      <c r="D53" s="8">
+        <v>43986</v>
+      </c>
+      <c r="E53" s="8">
         <v>43986</v>
       </c>
     </row>
@@ -2152,10 +2143,10 @@
       <c r="C55" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="D55" s="9">
-        <v>43986</v>
-      </c>
-      <c r="E55" s="9">
+      <c r="D55" s="8">
+        <v>43986</v>
+      </c>
+      <c r="E55" s="8">
         <v>43986</v>
       </c>
     </row>
@@ -2169,10 +2160,10 @@
       <c r="C56" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="D56" s="9">
-        <v>43986</v>
-      </c>
-      <c r="E56" s="9">
+      <c r="D56" s="8">
+        <v>43986</v>
+      </c>
+      <c r="E56" s="8">
         <v>43986</v>
       </c>
     </row>
@@ -2203,10 +2194,10 @@
       <c r="C58" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="D58" s="9">
-        <v>43986</v>
-      </c>
-      <c r="E58" s="9">
+      <c r="D58" s="8">
+        <v>43986</v>
+      </c>
+      <c r="E58" s="8">
         <v>43986</v>
       </c>
     </row>
@@ -2220,10 +2211,10 @@
       <c r="C59" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="D59" s="9">
-        <v>43986</v>
-      </c>
-      <c r="E59" s="9">
+      <c r="D59" s="8">
+        <v>43986</v>
+      </c>
+      <c r="E59" s="8">
         <v>43986</v>
       </c>
     </row>
@@ -2254,10 +2245,10 @@
       <c r="C61" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="D61" s="9">
-        <v>43986</v>
-      </c>
-      <c r="E61" s="9">
+      <c r="D61" s="8">
+        <v>43986</v>
+      </c>
+      <c r="E61" s="8">
         <v>43986</v>
       </c>
     </row>
@@ -2271,10 +2262,10 @@
       <c r="C62" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="D62" s="9">
-        <v>43986</v>
-      </c>
-      <c r="E62" s="9">
+      <c r="D62" s="8">
+        <v>43986</v>
+      </c>
+      <c r="E62" s="8">
         <v>43986</v>
       </c>
     </row>
@@ -2305,10 +2296,10 @@
       <c r="C64" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="D64" s="9">
-        <v>43986</v>
-      </c>
-      <c r="E64" s="9">
+      <c r="D64" s="8">
+        <v>43986</v>
+      </c>
+      <c r="E64" s="8">
         <v>43986</v>
       </c>
     </row>
@@ -2322,10 +2313,10 @@
       <c r="C65" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="D65" s="9">
-        <v>43986</v>
-      </c>
-      <c r="E65" s="9">
+      <c r="D65" s="8">
+        <v>43986</v>
+      </c>
+      <c r="E65" s="8">
         <v>43986</v>
       </c>
     </row>
@@ -2356,10 +2347,10 @@
       <c r="C67" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="D67" s="9">
-        <v>43986</v>
-      </c>
-      <c r="E67" s="9">
+      <c r="D67" s="8">
+        <v>43986</v>
+      </c>
+      <c r="E67" s="8">
         <v>43986</v>
       </c>
     </row>
@@ -2373,10 +2364,10 @@
       <c r="C68" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="D68" s="9">
-        <v>43986</v>
-      </c>
-      <c r="E68" s="9">
+      <c r="D68" s="8">
+        <v>43986</v>
+      </c>
+      <c r="E68" s="8">
         <v>43986</v>
       </c>
     </row>
@@ -2407,10 +2398,10 @@
       <c r="C70" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="D70" s="9">
-        <v>43986</v>
-      </c>
-      <c r="E70" s="9">
+      <c r="D70" s="8">
+        <v>43986</v>
+      </c>
+      <c r="E70" s="8">
         <v>43986</v>
       </c>
     </row>
@@ -2424,10 +2415,10 @@
       <c r="C71" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="D71" s="9">
-        <v>43986</v>
-      </c>
-      <c r="E71" s="9">
+      <c r="D71" s="8">
+        <v>43986</v>
+      </c>
+      <c r="E71" s="8">
         <v>43986</v>
       </c>
     </row>
@@ -2441,10 +2432,10 @@
       <c r="C72" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="D72" s="7">
+      <c r="D72" s="8">
         <v>43980</v>
       </c>
-      <c r="E72" s="7">
+      <c r="E72" s="8">
         <v>43980</v>
       </c>
     </row>
@@ -2458,10 +2449,10 @@
       <c r="C73" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="D73" s="9">
-        <v>43986</v>
-      </c>
-      <c r="E73" s="9">
+      <c r="D73" s="8">
+        <v>43986</v>
+      </c>
+      <c r="E73" s="8">
         <v>43986</v>
       </c>
     </row>
@@ -2475,10 +2466,10 @@
       <c r="C74" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="D74" s="9">
-        <v>43986</v>
-      </c>
-      <c r="E74" s="9">
+      <c r="D74" s="8">
+        <v>43986</v>
+      </c>
+      <c r="E74" s="8">
         <v>43986</v>
       </c>
     </row>
@@ -2492,10 +2483,10 @@
       <c r="C75" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="D75" s="7">
+      <c r="D75" s="8">
         <v>43980</v>
       </c>
-      <c r="E75" s="7">
+      <c r="E75" s="8">
         <v>43980</v>
       </c>
     </row>
@@ -2509,10 +2500,10 @@
       <c r="C76" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="D76" s="9">
-        <v>43986</v>
-      </c>
-      <c r="E76" s="9">
+      <c r="D76" s="8">
+        <v>43986</v>
+      </c>
+      <c r="E76" s="8">
         <v>43986</v>
       </c>
     </row>
@@ -2526,10 +2517,10 @@
       <c r="C77" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="D77" s="9">
-        <v>43986</v>
-      </c>
-      <c r="E77" s="9">
+      <c r="D77" s="8">
+        <v>43986</v>
+      </c>
+      <c r="E77" s="8">
         <v>43986</v>
       </c>
     </row>
@@ -2543,10 +2534,10 @@
       <c r="C78" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="D78" s="7">
+      <c r="D78" s="8">
         <v>43980</v>
       </c>
-      <c r="E78" s="7">
+      <c r="E78" s="8">
         <v>43980</v>
       </c>
     </row>
@@ -2560,10 +2551,10 @@
       <c r="C79" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="D79" s="9">
-        <v>43986</v>
-      </c>
-      <c r="E79" s="9">
+      <c r="D79" s="8">
+        <v>43986</v>
+      </c>
+      <c r="E79" s="8">
         <v>43986</v>
       </c>
     </row>
@@ -2577,10 +2568,10 @@
       <c r="C80" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="D80" s="9">
-        <v>43986</v>
-      </c>
-      <c r="E80" s="9">
+      <c r="D80" s="8">
+        <v>43986</v>
+      </c>
+      <c r="E80" s="8">
         <v>43986</v>
       </c>
     </row>
@@ -2594,10 +2585,10 @@
       <c r="C81" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="D81" s="7">
+      <c r="D81" s="8">
         <v>43980</v>
       </c>
-      <c r="E81" s="7">
+      <c r="E81" s="8">
         <v>43980</v>
       </c>
     </row>
@@ -2611,10 +2602,10 @@
       <c r="C82" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="D82" s="9">
-        <v>43986</v>
-      </c>
-      <c r="E82" s="9">
+      <c r="D82" s="8">
+        <v>43986</v>
+      </c>
+      <c r="E82" s="8">
         <v>43986</v>
       </c>
     </row>
@@ -2628,10 +2619,10 @@
       <c r="C83" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="D83" s="9">
-        <v>43986</v>
-      </c>
-      <c r="E83" s="9">
+      <c r="D83" s="8">
+        <v>43986</v>
+      </c>
+      <c r="E83" s="8">
         <v>43986</v>
       </c>
     </row>
@@ -2645,10 +2636,10 @@
       <c r="C84" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="D84" s="7">
+      <c r="D84" s="8">
         <v>43980</v>
       </c>
-      <c r="E84" s="7">
+      <c r="E84" s="8">
         <v>43980</v>
       </c>
     </row>
@@ -2662,10 +2653,10 @@
       <c r="C85" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="D85" s="9">
-        <v>43986</v>
-      </c>
-      <c r="E85" s="9">
+      <c r="D85" s="8">
+        <v>43986</v>
+      </c>
+      <c r="E85" s="8">
         <v>43986</v>
       </c>
     </row>
@@ -2679,10 +2670,10 @@
       <c r="C86" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="D86" s="9">
-        <v>43986</v>
-      </c>
-      <c r="E86" s="9">
+      <c r="D86" s="8">
+        <v>43986</v>
+      </c>
+      <c r="E86" s="8">
         <v>43986</v>
       </c>
     </row>
@@ -2696,10 +2687,10 @@
       <c r="C87" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="D87" s="7">
+      <c r="D87" s="8">
         <v>43980</v>
       </c>
-      <c r="E87" s="7">
+      <c r="E87" s="8">
         <v>43980</v>
       </c>
     </row>
@@ -2713,10 +2704,10 @@
       <c r="C88" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="D88" s="9">
-        <v>43986</v>
-      </c>
-      <c r="E88" s="9">
+      <c r="D88" s="8">
+        <v>43986</v>
+      </c>
+      <c r="E88" s="8">
         <v>43986</v>
       </c>
     </row>
@@ -2730,10 +2721,10 @@
       <c r="C89" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="D89" s="9">
-        <v>43986</v>
-      </c>
-      <c r="E89" s="9">
+      <c r="D89" s="8">
+        <v>43986</v>
+      </c>
+      <c r="E89" s="8">
         <v>43986</v>
       </c>
     </row>
@@ -2747,10 +2738,10 @@
       <c r="C90" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="D90" s="7">
+      <c r="D90" s="8">
         <v>43980</v>
       </c>
-      <c r="E90" s="7">
+      <c r="E90" s="8">
         <v>43980</v>
       </c>
     </row>
@@ -2764,10 +2755,10 @@
       <c r="C91" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="D91" s="9">
-        <v>43986</v>
-      </c>
-      <c r="E91" s="9">
+      <c r="D91" s="8">
+        <v>43986</v>
+      </c>
+      <c r="E91" s="8">
         <v>43986</v>
       </c>
     </row>
@@ -2781,10 +2772,10 @@
       <c r="C92" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="D92" s="9">
-        <v>43986</v>
-      </c>
-      <c r="E92" s="9">
+      <c r="D92" s="8">
+        <v>43986</v>
+      </c>
+      <c r="E92" s="8">
         <v>43986</v>
       </c>
     </row>
@@ -2798,10 +2789,10 @@
       <c r="C93" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="D93" s="7">
+      <c r="D93" s="8">
         <v>43980</v>
       </c>
-      <c r="E93" s="7">
+      <c r="E93" s="8">
         <v>43980</v>
       </c>
     </row>
@@ -2815,10 +2806,10 @@
       <c r="C94" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="D94" s="9">
-        <v>43986</v>
-      </c>
-      <c r="E94" s="9">
+      <c r="D94" s="8">
+        <v>43986</v>
+      </c>
+      <c r="E94" s="8">
         <v>43986</v>
       </c>
     </row>
@@ -2832,10 +2823,10 @@
       <c r="C95" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="D95" s="9">
-        <v>43986</v>
-      </c>
-      <c r="E95" s="9">
+      <c r="D95" s="8">
+        <v>43986</v>
+      </c>
+      <c r="E95" s="8">
         <v>43986</v>
       </c>
     </row>
@@ -2849,10 +2840,10 @@
       <c r="C96" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="D96" s="7">
+      <c r="D96" s="8">
         <v>43980</v>
       </c>
-      <c r="E96" s="7">
+      <c r="E96" s="8">
         <v>43980</v>
       </c>
     </row>
@@ -2866,10 +2857,10 @@
       <c r="C97" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="D97" s="9">
-        <v>43986</v>
-      </c>
-      <c r="E97" s="9">
+      <c r="D97" s="8">
+        <v>43986</v>
+      </c>
+      <c r="E97" s="8">
         <v>43986</v>
       </c>
     </row>
@@ -2883,10 +2874,10 @@
       <c r="C98" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="D98" s="9">
-        <v>43986</v>
-      </c>
-      <c r="E98" s="9">
+      <c r="D98" s="8">
+        <v>43986</v>
+      </c>
+      <c r="E98" s="8">
         <v>43986</v>
       </c>
     </row>
@@ -2900,10 +2891,10 @@
       <c r="C99" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="D99" s="9">
-        <v>43986</v>
-      </c>
-      <c r="E99" s="9">
+      <c r="D99" s="8">
+        <v>43986</v>
+      </c>
+      <c r="E99" s="8">
         <v>43986</v>
       </c>
     </row>
@@ -2917,10 +2908,10 @@
       <c r="C100" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="D100" s="9">
-        <v>43986</v>
-      </c>
-      <c r="E100" s="9">
+      <c r="D100" s="8">
+        <v>43986</v>
+      </c>
+      <c r="E100" s="8">
         <v>43986</v>
       </c>
     </row>
@@ -2934,10 +2925,10 @@
       <c r="C101" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="D101" s="9">
-        <v>43986</v>
-      </c>
-      <c r="E101" s="9">
+      <c r="D101" s="8">
+        <v>43986</v>
+      </c>
+      <c r="E101" s="8">
         <v>43986</v>
       </c>
     </row>
@@ -2951,10 +2942,10 @@
       <c r="C102" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="D102" s="9">
-        <v>43986</v>
-      </c>
-      <c r="E102" s="9">
+      <c r="D102" s="8">
+        <v>43986</v>
+      </c>
+      <c r="E102" s="8">
         <v>43986</v>
       </c>
     </row>
@@ -3177,7 +3168,7 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="9" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -3188,7 +3179,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="14"/>
+      <c r="A4" s="10"/>
       <c r="B4" s="3" t="s">
         <v>26</v>
       </c>
@@ -3197,7 +3188,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="14"/>
+      <c r="A5" s="10"/>
       <c r="B5" s="3" t="s">
         <v>27</v>
       </c>
@@ -3206,7 +3197,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="15"/>
+      <c r="A6" s="11"/>
       <c r="B6" s="3" t="s">
         <v>28</v>
       </c>
@@ -3215,7 +3206,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="9" t="s">
         <v>37</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -3226,7 +3217,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="14"/>
+      <c r="A9" s="10"/>
       <c r="B9" s="3" t="s">
         <v>39</v>
       </c>
@@ -3235,7 +3226,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="14"/>
+      <c r="A10" s="10"/>
       <c r="B10" s="3" t="s">
         <v>40</v>
       </c>
@@ -3244,7 +3235,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="15"/>
+      <c r="A11" s="11"/>
       <c r="B11" s="3" t="s">
         <v>41</v>
       </c>
@@ -3253,7 +3244,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="9" t="s">
         <v>47</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -3264,7 +3255,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="14"/>
+      <c r="A14" s="10"/>
       <c r="B14" s="3" t="s">
         <v>51</v>
       </c>
@@ -3273,7 +3264,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="14"/>
+      <c r="A15" s="10"/>
       <c r="B15" s="3" t="s">
         <v>52</v>
       </c>
@@ -3282,7 +3273,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="15"/>
+      <c r="A16" s="11"/>
       <c r="B16" s="3" t="s">
         <v>53</v>
       </c>
@@ -3291,7 +3282,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="9" t="s">
         <v>58</v>
       </c>
       <c r="B18" s="3" t="s">
@@ -3302,7 +3293,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="14"/>
+      <c r="A19" s="10"/>
       <c r="B19" s="3" t="s">
         <v>62</v>
       </c>
@@ -3311,7 +3302,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="14"/>
+      <c r="A20" s="10"/>
       <c r="B20" s="3" t="s">
         <v>63</v>
       </c>
@@ -3320,7 +3311,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="15"/>
+      <c r="A21" s="11"/>
       <c r="B21" s="3" t="s">
         <v>64</v>
       </c>
@@ -3329,7 +3320,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="9" t="s">
         <v>70</v>
       </c>
       <c r="B23" s="3" t="s">
@@ -3340,7 +3331,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24" s="14"/>
+      <c r="A24" s="10"/>
       <c r="B24" s="3" t="s">
         <v>79</v>
       </c>
@@ -3349,7 +3340,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A25" s="14"/>
+      <c r="A25" s="10"/>
       <c r="B25" s="3" t="s">
         <v>80</v>
       </c>
@@ -3358,7 +3349,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="15"/>
+      <c r="A26" s="11"/>
       <c r="B26" s="3" t="s">
         <v>81</v>
       </c>
@@ -3367,18 +3358,18 @@
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" s="16" t="s">
+      <c r="A28" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" s="17" t="s">
+      <c r="A30" s="16" t="s">
         <v>160</v>
       </c>
-      <c r="B30" s="17"/>
-      <c r="C30" s="17"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>